<commit_message>
2 tabs added to organize the nex buttons - Published in name of Pierre Lowe
</commit_message>
<xml_diff>
--- a/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
+++ b/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\01 DEPARTMENTS\04 SURVEY\09 PERSONAL WORK FOLDERS\Pierre\Online Log test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\PYTHON\Vicente\Online Log Development\Excel Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB70F86F-7B6B-44C2-8468-B2F5B0926C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ABAFF1A-ED8A-4226-89CF-26E247DD1699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{1722F03E-A338-4BDB-920F-BA87EA8992B5}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{1722F03E-A338-4BDB-920F-BA87EA8992B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16717" uniqueCount="16552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16730" uniqueCount="16559">
   <si>
     <t>Date</t>
   </si>
@@ -49692,6 +49692,27 @@
   </si>
   <si>
     <t>12;18;35.60307E</t>
+  </si>
+  <si>
+    <t>bae4511d-3b81-4efd-976c-62d0e0d457e7</t>
+  </si>
+  <si>
+    <t>0bdd6b73-cf40-4240-98a1-3beb59d89b9e</t>
+  </si>
+  <si>
+    <t>33a94533-52e6-4896-b89e-6b60a3ac22d2</t>
+  </si>
+  <si>
+    <t>9d524472-5bef-4e87-b11f-2ce0ed20ed39</t>
+  </si>
+  <si>
+    <t>a1068124-4055-4f81-a7df-19950e3fc719</t>
+  </si>
+  <si>
+    <t>c4d13ca7-d333-49b1-a9ee-df050d6cd010</t>
+  </si>
+  <si>
+    <t>23db5eba-3aea-4ecf-ae72-99e1499171b7</t>
   </si>
 </sst>
 </file>
@@ -50166,24 +50187,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E3A69F-5804-46B3-8092-81B33E8A06FF}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:XFD57"/>
+  <dimension ref="A1:XFD64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.44140625" customWidth="1"/>
-    <col min="6" max="6" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="101.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.36328125" style="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.453125" customWidth="1"/>
+    <col min="6" max="6" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="101.81640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="38.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16384" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -99337,7 +99358,7 @@
         <v>16382</v>
       </c>
     </row>
-    <row r="2" spans="1:16384" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16384" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="32">
         <v>45774</v>
       </c>
@@ -99378,7 +99399,7 @@
         <v>16395</v>
       </c>
     </row>
-    <row r="3" spans="1:16384" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16384" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="29">
         <v>45774</v>
       </c>
@@ -99419,7 +99440,7 @@
         <v>16398</v>
       </c>
     </row>
-    <row r="4" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="28">
         <v>45774</v>
       </c>
@@ -99451,7 +99472,7 @@
         <v>16401</v>
       </c>
     </row>
-    <row r="5" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="28">
         <v>45774</v>
       </c>
@@ -99483,7 +99504,7 @@
         <v>16404</v>
       </c>
     </row>
-    <row r="6" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="28">
         <v>45774</v>
       </c>
@@ -99518,7 +99539,7 @@
         <v>16406</v>
       </c>
     </row>
-    <row r="7" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="28">
         <v>45774</v>
       </c>
@@ -99550,7 +99571,7 @@
         <v>16409</v>
       </c>
     </row>
-    <row r="8" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="28">
         <v>45774</v>
       </c>
@@ -99585,7 +99606,7 @@
         <v>16412</v>
       </c>
     </row>
-    <row r="9" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="28">
         <v>45774</v>
       </c>
@@ -99617,7 +99638,7 @@
         <v>16415</v>
       </c>
     </row>
-    <row r="10" spans="1:16384" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16384" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="32">
         <v>45774</v>
       </c>
@@ -99658,7 +99679,7 @@
         <v>16420</v>
       </c>
     </row>
-    <row r="11" spans="1:16384" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16384" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="32">
         <v>45774</v>
       </c>
@@ -99699,7 +99720,7 @@
         <v>16423</v>
       </c>
     </row>
-    <row r="12" spans="1:16384" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16384" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="25">
         <v>45774</v>
       </c>
@@ -99740,7 +99761,7 @@
         <v>16428</v>
       </c>
     </row>
-    <row r="13" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="28">
         <v>45774</v>
       </c>
@@ -99772,7 +99793,7 @@
         <v>16431</v>
       </c>
     </row>
-    <row r="14" spans="1:16384" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16384" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="25">
         <v>45774</v>
       </c>
@@ -99813,7 +99834,7 @@
         <v>16434</v>
       </c>
     </row>
-    <row r="15" spans="1:16384" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16384" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="29">
         <v>45774</v>
       </c>
@@ -99854,7 +99875,7 @@
         <v>16437</v>
       </c>
     </row>
-    <row r="16" spans="1:16384" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16384" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="30">
         <v>45774</v>
       </c>
@@ -99895,7 +99916,7 @@
         <v>16440</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="32">
         <v>45774</v>
       </c>
@@ -99936,7 +99957,7 @@
         <v>16444</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="25">
         <v>45774</v>
       </c>
@@ -99977,7 +99998,7 @@
         <v>16447</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="29">
         <v>45774</v>
       </c>
@@ -100018,7 +100039,7 @@
         <v>16450</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="32">
         <v>45774</v>
       </c>
@@ -100059,7 +100080,7 @@
         <v>16453</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="25">
         <v>45774</v>
       </c>
@@ -100100,7 +100121,7 @@
         <v>16456</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="30">
         <v>45774</v>
       </c>
@@ -100141,7 +100162,7 @@
         <v>16458</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="25">
         <v>45774</v>
       </c>
@@ -100182,7 +100203,7 @@
         <v>16461</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="29">
         <v>45774</v>
       </c>
@@ -100223,7 +100244,7 @@
         <v>16465</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="30">
         <v>45774</v>
       </c>
@@ -100264,7 +100285,7 @@
         <v>16469</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="31">
         <v>45774</v>
       </c>
@@ -100305,7 +100326,7 @@
         <v>16472</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="30">
         <v>45774</v>
       </c>
@@ -100346,7 +100367,7 @@
         <v>16475</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="26">
         <v>45775</v>
       </c>
@@ -100384,7 +100405,7 @@
         <v>16478</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="27">
         <v>45775</v>
       </c>
@@ -100422,7 +100443,7 @@
         <v>16483</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="24">
         <v>45775</v>
       </c>
@@ -100457,7 +100478,7 @@
         <v>16488</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="32">
         <v>45775</v>
       </c>
@@ -100498,7 +100519,7 @@
         <v>16492</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="25">
         <v>45775</v>
       </c>
@@ -100539,7 +100560,7 @@
         <v>16497</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="28">
         <v>45775</v>
       </c>
@@ -100571,7 +100592,7 @@
         <v>16501</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="30">
         <v>45775</v>
       </c>
@@ -100612,7 +100633,7 @@
         <v>16505</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="32">
         <v>45776</v>
       </c>
@@ -100633,7 +100654,7 @@
         <v>16509</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="25">
         <v>45776</v>
       </c>
@@ -100654,7 +100675,7 @@
         <v>16510</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="32">
         <v>45776</v>
       </c>
@@ -100675,7 +100696,7 @@
         <v>16511</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="32">
         <v>45776</v>
       </c>
@@ -100696,7 +100717,7 @@
         <v>16512</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="32">
         <v>45776</v>
       </c>
@@ -100719,7 +100740,7 @@
         <v>16513</v>
       </c>
     </row>
-    <row r="40" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="25">
         <v>45776</v>
       </c>
@@ -100742,7 +100763,7 @@
         <v>16514</v>
       </c>
     </row>
-    <row r="41" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="32">
         <v>45776</v>
       </c>
@@ -100765,7 +100786,7 @@
         <v>16515</v>
       </c>
     </row>
-    <row r="42" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="32">
         <v>45776</v>
       </c>
@@ -100788,7 +100809,7 @@
         <v>16516</v>
       </c>
     </row>
-    <row r="43" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="25">
         <v>45776</v>
       </c>
@@ -100811,7 +100832,7 @@
         <v>16517</v>
       </c>
     </row>
-    <row r="44" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="32">
         <v>45811</v>
       </c>
@@ -100834,7 +100855,7 @@
         <v>16518</v>
       </c>
     </row>
-    <row r="45" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="25">
         <v>45811</v>
       </c>
@@ -100857,7 +100878,7 @@
         <v>16521</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="24">
         <v>45811</v>
       </c>
@@ -100871,7 +100892,7 @@
         <v>16522</v>
       </c>
     </row>
-    <row r="47" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="30">
         <v>45811</v>
       </c>
@@ -100894,7 +100915,7 @@
         <v>16523</v>
       </c>
     </row>
-    <row r="48" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="29">
         <v>45812</v>
       </c>
@@ -100935,7 +100956,7 @@
         <v>16526</v>
       </c>
     </row>
-    <row r="49" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="29">
         <v>45812</v>
       </c>
@@ -100973,7 +100994,7 @@
         <v>16528</v>
       </c>
     </row>
-    <row r="50" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="32">
         <v>45812</v>
       </c>
@@ -101014,7 +101035,7 @@
         <v>16533</v>
       </c>
     </row>
-    <row r="51" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="25">
         <v>45812</v>
       </c>
@@ -101055,7 +101076,7 @@
         <v>16536</v>
       </c>
     </row>
-    <row r="52" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="30">
         <v>45812</v>
       </c>
@@ -101096,7 +101117,7 @@
         <v>16538</v>
       </c>
     </row>
-    <row r="53" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="30">
         <v>45812</v>
       </c>
@@ -101137,7 +101158,7 @@
         <v>16540</v>
       </c>
     </row>
-    <row r="54" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="31">
         <v>45812</v>
       </c>
@@ -101178,7 +101199,7 @@
         <v>16542</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="24">
         <v>45812</v>
       </c>
@@ -101219,7 +101240,7 @@
         <v>16544</v>
       </c>
     </row>
-    <row r="56" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="29">
         <v>45812</v>
       </c>
@@ -101260,7 +101281,7 @@
         <v>16547</v>
       </c>
     </row>
-    <row r="57" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="28">
         <v>45812</v>
       </c>
@@ -101290,6 +101311,101 @@
       </c>
       <c r="Q57" s="33" t="s">
         <v>16549</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="26">
+        <v>45812</v>
+      </c>
+      <c r="B58" s="5">
+        <v>0.84152777777777776</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>16383</v>
+      </c>
+      <c r="Q58" s="36" t="s">
+        <v>16552</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="27">
+        <v>45812</v>
+      </c>
+      <c r="B59" s="7">
+        <v>0.84156249999999999</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>16384</v>
+      </c>
+      <c r="Q59" s="37" t="s">
+        <v>16553</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="29">
+        <v>45812</v>
+      </c>
+      <c r="B60" s="11">
+        <v>0.84165509259259264</v>
+      </c>
+      <c r="E60" s="12" t="s">
+        <v>16387</v>
+      </c>
+      <c r="Q60" s="22" t="s">
+        <v>16554</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="26">
+        <v>45814</v>
+      </c>
+      <c r="B61" s="5">
+        <v>0.77491898148148153</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>16383</v>
+      </c>
+      <c r="Q61" s="36" t="s">
+        <v>16555</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="27">
+        <v>45814</v>
+      </c>
+      <c r="B62" s="7">
+        <v>0.77510416666666671</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>16384</v>
+      </c>
+      <c r="Q62" s="37" t="s">
+        <v>16556</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="28">
+        <v>45814</v>
+      </c>
+      <c r="B63" s="9">
+        <v>0.77512731481481478</v>
+      </c>
+      <c r="Q63" s="33" t="s">
+        <v>16557</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="29">
+        <v>45814</v>
+      </c>
+      <c r="B64" s="11">
+        <v>0.77523148148148147</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>16387</v>
+      </c>
+      <c r="Q64" s="22" t="s">
+        <v>16558</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Open settings menu in the startup
</commit_message>
<xml_diff>
--- a/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
+++ b/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\PYTHON\Vicente\Online Log Development\Excel Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ABAFF1A-ED8A-4226-89CF-26E247DD1699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F694BDBB-E6C5-44B4-8282-F9B98A3F163B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{1722F03E-A338-4BDB-920F-BA87EA8992B5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16730" uniqueCount="16559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16732" uniqueCount="16561">
   <si>
     <t>Date</t>
   </si>
@@ -49713,6 +49713,12 @@
   </si>
   <si>
     <t>23db5eba-3aea-4ecf-ae72-99e1499171b7</t>
+  </si>
+  <si>
+    <t>79de45a9-1afa-46a0-82ea-c370fd27fb7b</t>
+  </si>
+  <si>
+    <t>CustomS2 1 Event</t>
   </si>
 </sst>
 </file>
@@ -49739,7 +49745,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -49800,6 +49806,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBAFFC9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -49813,7 +49825,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -49852,6 +49864,10 @@
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="21" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -50187,7 +50203,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E3A69F-5804-46B3-8092-81B33E8A06FF}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:XFD64"/>
+  <dimension ref="A1:XFD65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
@@ -101408,6 +101424,20 @@
         <v>16558</v>
       </c>
     </row>
+    <row r="65" spans="1:17" s="40" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="38">
+        <v>45814</v>
+      </c>
+      <c r="B65" s="39">
+        <v>0.83177083333333335</v>
+      </c>
+      <c r="E65" s="40" t="s">
+        <v>16560</v>
+      </c>
+      <c r="Q65" s="41" t="s">
+        <v>16559</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Improved documentation for _perform_log_action() and insert_txt_data()
</commit_message>
<xml_diff>
--- a/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
+++ b/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\PYTHON\Vicente\Online Log Development\Excel Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F694BDBB-E6C5-44B4-8282-F9B98A3F163B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F3AE60-C54B-4F3D-85C2-3ACE1333C008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{1722F03E-A338-4BDB-920F-BA87EA8992B5}"/>
+    <workbookView xWindow="8060" yWindow="3080" windowWidth="32140" windowHeight="16720" xr2:uid="{1722F03E-A338-4BDB-920F-BA87EA8992B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16732" uniqueCount="16561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16750" uniqueCount="16571">
   <si>
     <t>Date</t>
   </si>
@@ -49719,6 +49719,36 @@
   </si>
   <si>
     <t>CustomS2 1 Event</t>
+  </si>
+  <si>
+    <t>520cc050-1c8a-4d44-af8c-929cd3506ce9</t>
+  </si>
+  <si>
+    <t>19cb0508-d99e-469c-ae32-f3d08e3af861</t>
+  </si>
+  <si>
+    <t>1853db29-9337-48ce-870f-849b875395db</t>
+  </si>
+  <si>
+    <t>39d8b35d-1708-4fa1-a639-63707827da40</t>
+  </si>
+  <si>
+    <t>2f7058d2-e7c9-4276-913b-ed3a10ba963c</t>
+  </si>
+  <si>
+    <t>f1b929e7-3faa-4d01-a34f-c0500b006aef</t>
+  </si>
+  <si>
+    <t>Custom 1 Event</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>1e4d5ab8-6a6b-4329-9a03-e95a78827cfe</t>
+  </si>
+  <si>
+    <t>9cd5a561-236b-4d3c-b39a-9804700195ab</t>
   </si>
 </sst>
 </file>
@@ -50203,7 +50233,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E3A69F-5804-46B3-8092-81B33E8A06FF}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:XFD65"/>
+  <dimension ref="A1:XFD73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
@@ -101438,6 +101468,124 @@
         <v>16559</v>
       </c>
     </row>
+    <row r="66" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="29">
+        <v>45815</v>
+      </c>
+      <c r="B66" s="11">
+        <v>1.1574074074074073E-5</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>16387</v>
+      </c>
+      <c r="Q66" s="22" t="s">
+        <v>16561</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="27">
+        <v>45815</v>
+      </c>
+      <c r="B67" s="7">
+        <v>0.50662037037037033</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>16384</v>
+      </c>
+      <c r="Q67" s="37" t="s">
+        <v>16562</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="26">
+        <v>45815</v>
+      </c>
+      <c r="B68" s="5">
+        <v>0.50850694444444444</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>16383</v>
+      </c>
+      <c r="Q68" s="36" t="s">
+        <v>16563</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="27">
+        <v>45815</v>
+      </c>
+      <c r="B69" s="7">
+        <v>0.50855324074074071</v>
+      </c>
+      <c r="E69" s="8" t="s">
+        <v>16384</v>
+      </c>
+      <c r="Q69" s="37" t="s">
+        <v>16564</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="28">
+        <v>45815</v>
+      </c>
+      <c r="B70" s="9">
+        <v>0.5085763888888889</v>
+      </c>
+      <c r="Q70" s="33" t="s">
+        <v>16565</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A71" s="24">
+        <v>45815</v>
+      </c>
+      <c r="B71" s="2">
+        <v>0.51571759259259264</v>
+      </c>
+      <c r="E71" t="s">
+        <v>16567</v>
+      </c>
+      <c r="G71" t="s">
+        <v>16568</v>
+      </c>
+      <c r="Q71" s="19" t="s">
+        <v>16566</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="26">
+        <v>45815</v>
+      </c>
+      <c r="B72" s="5">
+        <v>0.51863425925925921</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>16383</v>
+      </c>
+      <c r="G72" s="6" t="s">
+        <v>16568</v>
+      </c>
+      <c r="Q72" s="36" t="s">
+        <v>16569</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="27">
+        <v>45815</v>
+      </c>
+      <c r="B73" s="7">
+        <v>0.51869212962962963</v>
+      </c>
+      <c r="E73" s="8" t="s">
+        <v>16384</v>
+      </c>
+      <c r="G73" s="8" t="s">
+        <v>16568</v>
+      </c>
+      <c r="Q73" s="37" t="s">
+        <v>16570</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Improved documentation and identation in DataLoggerGUI class
</commit_message>
<xml_diff>
--- a/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
+++ b/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\PYTHON\Vicente\Online Log Development\Excel Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F3AE60-C54B-4F3D-85C2-3ACE1333C008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1E13FC-2D13-45EA-8B13-7F34D85B9CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8060" yWindow="3080" windowWidth="32140" windowHeight="16720" xr2:uid="{1722F03E-A338-4BDB-920F-BA87EA8992B5}"/>
+    <workbookView xWindow="11740" yWindow="2610" windowWidth="32140" windowHeight="16720" xr2:uid="{1722F03E-A338-4BDB-920F-BA87EA8992B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16750" uniqueCount="16571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16763" uniqueCount="16578">
   <si>
     <t>Date</t>
   </si>
@@ -49749,6 +49749,27 @@
   </si>
   <si>
     <t>9cd5a561-236b-4d3c-b39a-9804700195ab</t>
+  </si>
+  <si>
+    <t>75dcdb6b-c465-4cc9-b6b4-c3d7f8eb082c</t>
+  </si>
+  <si>
+    <t>8d789724-5d54-40e0-a069-1a347e0812d7</t>
+  </si>
+  <si>
+    <t>912f8ac1-ff12-45ca-8a3b-4f1b33f5c18a</t>
+  </si>
+  <si>
+    <t>c7d955eb-e618-4a9f-ae64-39ac5a4f1556</t>
+  </si>
+  <si>
+    <t>67d08a6a-22ca-4f95-9b6a-aae655208b04</t>
+  </si>
+  <si>
+    <t>39159ff0-2489-4037-b2e3-30e60fac471a</t>
+  </si>
+  <si>
+    <t>5d88764c-a6df-4243-936f-6f07bfe771ff</t>
   </si>
 </sst>
 </file>
@@ -50233,11 +50254,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E3A69F-5804-46B3-8092-81B33E8A06FF}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:XFD73"/>
+  <dimension ref="A1:XFD80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E52" sqref="E52"/>
+      <selection pane="bottomLeft" activeCell="C74" sqref="C74:D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -101586,6 +101607,101 @@
         <v>16570</v>
       </c>
     </row>
+    <row r="74" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="26">
+        <v>45815</v>
+      </c>
+      <c r="B74" s="5">
+        <v>0.6885648148148148</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>16383</v>
+      </c>
+      <c r="Q74" s="36" t="s">
+        <v>16571</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="26">
+        <v>45815</v>
+      </c>
+      <c r="B75" s="5">
+        <v>0.7053356481481482</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>16383</v>
+      </c>
+      <c r="Q75" s="36" t="s">
+        <v>16572</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="29">
+        <v>45815</v>
+      </c>
+      <c r="B76" s="11">
+        <v>0.70549768518518519</v>
+      </c>
+      <c r="E76" s="12" t="s">
+        <v>16387</v>
+      </c>
+      <c r="Q76" s="22" t="s">
+        <v>16573</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="27">
+        <v>45815</v>
+      </c>
+      <c r="B77" s="7">
+        <v>0.70552083333333337</v>
+      </c>
+      <c r="E77" s="8" t="s">
+        <v>16384</v>
+      </c>
+      <c r="Q77" s="37" t="s">
+        <v>16574</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="28">
+        <v>45815</v>
+      </c>
+      <c r="B78" s="9">
+        <v>0.70553240740740741</v>
+      </c>
+      <c r="Q78" s="33" t="s">
+        <v>16575</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="26">
+        <v>45815</v>
+      </c>
+      <c r="B79" s="5">
+        <v>0.70554398148148145</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>16383</v>
+      </c>
+      <c r="Q79" s="36" t="s">
+        <v>16576</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="27">
+        <v>45815</v>
+      </c>
+      <c r="B80" s="7">
+        <v>0.70554398148148145</v>
+      </c>
+      <c r="E80" s="8" t="s">
+        <v>16384</v>
+      </c>
+      <c r="Q80" s="37" t="s">
+        <v>16577</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
-New Verison With button group layouts. - custom buttons can be assigned a attribute which places them into the attribute tab
-Function does not work correctly as when you press a custom button, nothing is written to the excel doc

-Log on, Log off, etc buttons no longer fill in event column in excel but do trigger an event from the associated text file
</commit_message>
<xml_diff>
--- a/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
+++ b/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\PYTHON\Vicente\Online Log Development\Excel Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\PYTHON\Online-Log-Development\Excel TEmplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1E13FC-2D13-45EA-8B13-7F34D85B9CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F02BB2C-D6EC-4245-AA49-24BA3D200D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11740" yWindow="2610" windowWidth="32140" windowHeight="16720" xr2:uid="{1722F03E-A338-4BDB-920F-BA87EA8992B5}"/>
+    <workbookView xWindow="45972" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{1722F03E-A338-4BDB-920F-BA87EA8992B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16763" uniqueCount="16578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16795" uniqueCount="16589">
   <si>
     <t>Date</t>
   </si>
@@ -49770,6 +49770,39 @@
   </si>
   <si>
     <t>5d88764c-a6df-4243-936f-6f07bfe771ff</t>
+  </si>
+  <si>
+    <t>e1a3db0b-9939-438b-9d08-23a917b754bf</t>
+  </si>
+  <si>
+    <t>a0544af1-a241-4701-b454-cca20bc5eef2</t>
+  </si>
+  <si>
+    <t>f15bbdde-31b3-4317-ac7c-9b76508218c7</t>
+  </si>
+  <si>
+    <t>B08_0310_0316_0314_S 2.00</t>
+  </si>
+  <si>
+    <t>54;24;02.67784N</t>
+  </si>
+  <si>
+    <t>12;18;37.61874E</t>
+  </si>
+  <si>
+    <t>d4f5e2ad-bd26-4edf-9cb6-32a4ab0b862a</t>
+  </si>
+  <si>
+    <t>48411929-405f-48cd-ae48-899f8cc04220</t>
+  </si>
+  <si>
+    <t>1ea7b835-85c7-48cd-a174-425aa86ec196</t>
+  </si>
+  <si>
+    <t>0b712172-e172-4f34-a0d6-af9ba43673c8</t>
+  </si>
+  <si>
+    <t>c5a637af-8aa7-42ee-b8e8-9ba48a3337dd</t>
   </si>
 </sst>
 </file>
@@ -50254,24 +50287,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E3A69F-5804-46B3-8092-81B33E8A06FF}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:XFD80"/>
+  <dimension ref="A1:XFD88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C74" sqref="C74:D74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.453125" customWidth="1"/>
-    <col min="6" max="6" width="29.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="101.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.44140625" customWidth="1"/>
+    <col min="6" max="6" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="101.77734375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="38.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="38.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16384" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -99425,7 +99458,7 @@
         <v>16382</v>
       </c>
     </row>
-    <row r="2" spans="1:16384" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16384" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="32">
         <v>45774</v>
       </c>
@@ -99466,7 +99499,7 @@
         <v>16395</v>
       </c>
     </row>
-    <row r="3" spans="1:16384" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16384" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29">
         <v>45774</v>
       </c>
@@ -99507,7 +99540,7 @@
         <v>16398</v>
       </c>
     </row>
-    <row r="4" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="28">
         <v>45774</v>
       </c>
@@ -99539,7 +99572,7 @@
         <v>16401</v>
       </c>
     </row>
-    <row r="5" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="28">
         <v>45774</v>
       </c>
@@ -99571,7 +99604,7 @@
         <v>16404</v>
       </c>
     </row>
-    <row r="6" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="28">
         <v>45774</v>
       </c>
@@ -99606,7 +99639,7 @@
         <v>16406</v>
       </c>
     </row>
-    <row r="7" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="28">
         <v>45774</v>
       </c>
@@ -99638,7 +99671,7 @@
         <v>16409</v>
       </c>
     </row>
-    <row r="8" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28">
         <v>45774</v>
       </c>
@@ -99673,7 +99706,7 @@
         <v>16412</v>
       </c>
     </row>
-    <row r="9" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="28">
         <v>45774</v>
       </c>
@@ -99705,7 +99738,7 @@
         <v>16415</v>
       </c>
     </row>
-    <row r="10" spans="1:16384" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16384" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="32">
         <v>45774</v>
       </c>
@@ -99746,7 +99779,7 @@
         <v>16420</v>
       </c>
     </row>
-    <row r="11" spans="1:16384" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16384" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="32">
         <v>45774</v>
       </c>
@@ -99787,7 +99820,7 @@
         <v>16423</v>
       </c>
     </row>
-    <row r="12" spans="1:16384" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16384" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="25">
         <v>45774</v>
       </c>
@@ -99828,7 +99861,7 @@
         <v>16428</v>
       </c>
     </row>
-    <row r="13" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="28">
         <v>45774</v>
       </c>
@@ -99860,7 +99893,7 @@
         <v>16431</v>
       </c>
     </row>
-    <row r="14" spans="1:16384" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16384" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25">
         <v>45774</v>
       </c>
@@ -99901,7 +99934,7 @@
         <v>16434</v>
       </c>
     </row>
-    <row r="15" spans="1:16384" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16384" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="29">
         <v>45774</v>
       </c>
@@ -99942,7 +99975,7 @@
         <v>16437</v>
       </c>
     </row>
-    <row r="16" spans="1:16384" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16384" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30">
         <v>45774</v>
       </c>
@@ -99983,7 +100016,7 @@
         <v>16440</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="32">
         <v>45774</v>
       </c>
@@ -100024,7 +100057,7 @@
         <v>16444</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="25">
         <v>45774</v>
       </c>
@@ -100065,7 +100098,7 @@
         <v>16447</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="29">
         <v>45774</v>
       </c>
@@ -100106,7 +100139,7 @@
         <v>16450</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="32">
         <v>45774</v>
       </c>
@@ -100147,7 +100180,7 @@
         <v>16453</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="25">
         <v>45774</v>
       </c>
@@ -100188,7 +100221,7 @@
         <v>16456</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="30">
         <v>45774</v>
       </c>
@@ -100229,7 +100262,7 @@
         <v>16458</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="25">
         <v>45774</v>
       </c>
@@ -100270,7 +100303,7 @@
         <v>16461</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="29">
         <v>45774</v>
       </c>
@@ -100311,7 +100344,7 @@
         <v>16465</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="30">
         <v>45774</v>
       </c>
@@ -100352,7 +100385,7 @@
         <v>16469</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="31">
         <v>45774</v>
       </c>
@@ -100393,7 +100426,7 @@
         <v>16472</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="30">
         <v>45774</v>
       </c>
@@ -100434,7 +100467,7 @@
         <v>16475</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="26">
         <v>45775</v>
       </c>
@@ -100472,7 +100505,7 @@
         <v>16478</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="27">
         <v>45775</v>
       </c>
@@ -100510,7 +100543,7 @@
         <v>16483</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="24">
         <v>45775</v>
       </c>
@@ -100545,7 +100578,7 @@
         <v>16488</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="32">
         <v>45775</v>
       </c>
@@ -100586,7 +100619,7 @@
         <v>16492</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="25">
         <v>45775</v>
       </c>
@@ -100627,7 +100660,7 @@
         <v>16497</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="28">
         <v>45775</v>
       </c>
@@ -100659,7 +100692,7 @@
         <v>16501</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="30">
         <v>45775</v>
       </c>
@@ -100700,7 +100733,7 @@
         <v>16505</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="32">
         <v>45776</v>
       </c>
@@ -100721,7 +100754,7 @@
         <v>16509</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="25">
         <v>45776</v>
       </c>
@@ -100742,7 +100775,7 @@
         <v>16510</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="32">
         <v>45776</v>
       </c>
@@ -100763,7 +100796,7 @@
         <v>16511</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="32">
         <v>45776</v>
       </c>
@@ -100784,7 +100817,7 @@
         <v>16512</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="32">
         <v>45776</v>
       </c>
@@ -100807,7 +100840,7 @@
         <v>16513</v>
       </c>
     </row>
-    <row r="40" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="25">
         <v>45776</v>
       </c>
@@ -100830,7 +100863,7 @@
         <v>16514</v>
       </c>
     </row>
-    <row r="41" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="32">
         <v>45776</v>
       </c>
@@ -100853,7 +100886,7 @@
         <v>16515</v>
       </c>
     </row>
-    <row r="42" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="32">
         <v>45776</v>
       </c>
@@ -100876,7 +100909,7 @@
         <v>16516</v>
       </c>
     </row>
-    <row r="43" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="25">
         <v>45776</v>
       </c>
@@ -100899,7 +100932,7 @@
         <v>16517</v>
       </c>
     </row>
-    <row r="44" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="32">
         <v>45811</v>
       </c>
@@ -100922,7 +100955,7 @@
         <v>16518</v>
       </c>
     </row>
-    <row r="45" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="25">
         <v>45811</v>
       </c>
@@ -100945,7 +100978,7 @@
         <v>16521</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="24">
         <v>45811</v>
       </c>
@@ -100959,7 +100992,7 @@
         <v>16522</v>
       </c>
     </row>
-    <row r="47" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="30">
         <v>45811</v>
       </c>
@@ -100982,7 +101015,7 @@
         <v>16523</v>
       </c>
     </row>
-    <row r="48" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="29">
         <v>45812</v>
       </c>
@@ -101023,7 +101056,7 @@
         <v>16526</v>
       </c>
     </row>
-    <row r="49" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="29">
         <v>45812</v>
       </c>
@@ -101061,7 +101094,7 @@
         <v>16528</v>
       </c>
     </row>
-    <row r="50" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="32">
         <v>45812</v>
       </c>
@@ -101102,7 +101135,7 @@
         <v>16533</v>
       </c>
     </row>
-    <row r="51" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="25">
         <v>45812</v>
       </c>
@@ -101143,7 +101176,7 @@
         <v>16536</v>
       </c>
     </row>
-    <row r="52" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="30">
         <v>45812</v>
       </c>
@@ -101184,7 +101217,7 @@
         <v>16538</v>
       </c>
     </row>
-    <row r="53" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="30">
         <v>45812</v>
       </c>
@@ -101225,7 +101258,7 @@
         <v>16540</v>
       </c>
     </row>
-    <row r="54" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="31">
         <v>45812</v>
       </c>
@@ -101266,7 +101299,7 @@
         <v>16542</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="24">
         <v>45812</v>
       </c>
@@ -101307,7 +101340,7 @@
         <v>16544</v>
       </c>
     </row>
-    <row r="56" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="29">
         <v>45812</v>
       </c>
@@ -101348,7 +101381,7 @@
         <v>16547</v>
       </c>
     </row>
-    <row r="57" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="28">
         <v>45812</v>
       </c>
@@ -101380,7 +101413,7 @@
         <v>16549</v>
       </c>
     </row>
-    <row r="58" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="26">
         <v>45812</v>
       </c>
@@ -101394,7 +101427,7 @@
         <v>16552</v>
       </c>
     </row>
-    <row r="59" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="27">
         <v>45812</v>
       </c>
@@ -101408,7 +101441,7 @@
         <v>16553</v>
       </c>
     </row>
-    <row r="60" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="29">
         <v>45812</v>
       </c>
@@ -101422,7 +101455,7 @@
         <v>16554</v>
       </c>
     </row>
-    <row r="61" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="26">
         <v>45814</v>
       </c>
@@ -101436,7 +101469,7 @@
         <v>16555</v>
       </c>
     </row>
-    <row r="62" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="27">
         <v>45814</v>
       </c>
@@ -101450,7 +101483,7 @@
         <v>16556</v>
       </c>
     </row>
-    <row r="63" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="28">
         <v>45814</v>
       </c>
@@ -101461,7 +101494,7 @@
         <v>16557</v>
       </c>
     </row>
-    <row r="64" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="29">
         <v>45814</v>
       </c>
@@ -101475,7 +101508,7 @@
         <v>16558</v>
       </c>
     </row>
-    <row r="65" spans="1:17" s="40" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:17" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="38">
         <v>45814</v>
       </c>
@@ -101489,7 +101522,7 @@
         <v>16559</v>
       </c>
     </row>
-    <row r="66" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="29">
         <v>45815</v>
       </c>
@@ -101503,7 +101536,7 @@
         <v>16561</v>
       </c>
     </row>
-    <row r="67" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="27">
         <v>45815</v>
       </c>
@@ -101517,7 +101550,7 @@
         <v>16562</v>
       </c>
     </row>
-    <row r="68" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="26">
         <v>45815</v>
       </c>
@@ -101531,7 +101564,7 @@
         <v>16563</v>
       </c>
     </row>
-    <row r="69" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="27">
         <v>45815</v>
       </c>
@@ -101545,7 +101578,7 @@
         <v>16564</v>
       </c>
     </row>
-    <row r="70" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="28">
         <v>45815</v>
       </c>
@@ -101556,7 +101589,7 @@
         <v>16565</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="24">
         <v>45815</v>
       </c>
@@ -101573,7 +101606,7 @@
         <v>16566</v>
       </c>
     </row>
-    <row r="72" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="26">
         <v>45815</v>
       </c>
@@ -101590,7 +101623,7 @@
         <v>16569</v>
       </c>
     </row>
-    <row r="73" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="27">
         <v>45815</v>
       </c>
@@ -101607,7 +101640,7 @@
         <v>16570</v>
       </c>
     </row>
-    <row r="74" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="26">
         <v>45815</v>
       </c>
@@ -101621,7 +101654,7 @@
         <v>16571</v>
       </c>
     </row>
-    <row r="75" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="26">
         <v>45815</v>
       </c>
@@ -101635,7 +101668,7 @@
         <v>16572</v>
       </c>
     </row>
-    <row r="76" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="29">
         <v>45815</v>
       </c>
@@ -101649,7 +101682,7 @@
         <v>16573</v>
       </c>
     </row>
-    <row r="77" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="27">
         <v>45815</v>
       </c>
@@ -101663,7 +101696,7 @@
         <v>16574</v>
       </c>
     </row>
-    <row r="78" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="28">
         <v>45815</v>
       </c>
@@ -101674,7 +101707,7 @@
         <v>16575</v>
       </c>
     </row>
-    <row r="79" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="26">
         <v>45815</v>
       </c>
@@ -101688,7 +101721,7 @@
         <v>16576</v>
       </c>
     </row>
-    <row r="80" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="27">
         <v>45815</v>
       </c>
@@ -101700,6 +101733,238 @@
       </c>
       <c r="Q80" s="37" t="s">
         <v>16577</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="26">
+        <v>45816</v>
+      </c>
+      <c r="B81" s="5">
+        <v>0.57025462962962958</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>16383</v>
+      </c>
+      <c r="Q81" s="36" t="s">
+        <v>16578</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="27">
+        <v>45816</v>
+      </c>
+      <c r="B82" s="7">
+        <v>0.57027777777777777</v>
+      </c>
+      <c r="E82" s="8" t="s">
+        <v>16384</v>
+      </c>
+      <c r="Q82" s="37" t="s">
+        <v>16579</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="26">
+        <v>45816</v>
+      </c>
+      <c r="B83" s="5">
+        <v>0.57039351851851849</v>
+      </c>
+      <c r="C83" s="6">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D83" s="6">
+        <v>-0.06</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>16383</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M83" s="6" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N83" s="6" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O83" s="6">
+        <v>325419.44</v>
+      </c>
+      <c r="P83" s="6">
+        <v>6031442.8799999999</v>
+      </c>
+      <c r="Q83" s="36" t="s">
+        <v>16580</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="27">
+        <v>45816</v>
+      </c>
+      <c r="B84" s="7">
+        <v>0.57041666666666668</v>
+      </c>
+      <c r="C84" s="8">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D84" s="8">
+        <v>-0.06</v>
+      </c>
+      <c r="E84" s="8" t="s">
+        <v>16384</v>
+      </c>
+      <c r="F84" s="8" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M84" s="8" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N84" s="8" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O84" s="8">
+        <v>325419.44</v>
+      </c>
+      <c r="P84" s="8">
+        <v>6031442.8799999999</v>
+      </c>
+      <c r="Q84" s="37" t="s">
+        <v>16584</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="26">
+        <v>45816</v>
+      </c>
+      <c r="B85" s="5">
+        <v>0.57054398148148144</v>
+      </c>
+      <c r="C85" s="6">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D85" s="6">
+        <v>-0.06</v>
+      </c>
+      <c r="E85" s="6" t="s">
+        <v>16383</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M85" s="6" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N85" s="6" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O85" s="6">
+        <v>325419.44</v>
+      </c>
+      <c r="P85" s="6">
+        <v>6031442.8799999999</v>
+      </c>
+      <c r="Q85" s="36" t="s">
+        <v>16585</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="27">
+        <v>45816</v>
+      </c>
+      <c r="B86" s="7">
+        <v>0.5706134259259259</v>
+      </c>
+      <c r="C86" s="8">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D86" s="8">
+        <v>-0.06</v>
+      </c>
+      <c r="E86" s="8" t="s">
+        <v>16384</v>
+      </c>
+      <c r="F86" s="8" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M86" s="8" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N86" s="8" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O86" s="8">
+        <v>325419.44</v>
+      </c>
+      <c r="P86" s="8">
+        <v>6031442.8799999999</v>
+      </c>
+      <c r="Q86" s="37" t="s">
+        <v>16586</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="26">
+        <v>45816</v>
+      </c>
+      <c r="B87" s="5">
+        <v>0.57451388888888888</v>
+      </c>
+      <c r="C87" s="6">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D87" s="6">
+        <v>-0.06</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M87" s="6" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N87" s="6" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O87" s="6">
+        <v>325419.44</v>
+      </c>
+      <c r="P87" s="6">
+        <v>6031442.8799999999</v>
+      </c>
+      <c r="Q87" s="36" t="s">
+        <v>16587</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="27">
+        <v>45816</v>
+      </c>
+      <c r="B88" s="7">
+        <v>0.57456018518518515</v>
+      </c>
+      <c r="C88" s="8">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D88" s="8">
+        <v>-0.06</v>
+      </c>
+      <c r="F88" s="8" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M88" s="8" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N88" s="8" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O88" s="8">
+        <v>325419.44</v>
+      </c>
+      <c r="P88" s="8">
+        <v>6031442.8799999999</v>
+      </c>
+      <c r="Q88" s="37" t="s">
+        <v>16588</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-Rev 16 has a function to group the layout of the custom buttons - this is done with new attribute to each button to place them into a group which are then grouped into tabs - currently merging with changes in Rev15
</commit_message>
<xml_diff>
--- a/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
+++ b/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\PYTHON\Online-Log-Development\Excel TEmplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F02BB2C-D6EC-4245-AA49-24BA3D200D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C88608B-B675-450F-88ED-BD25692C1272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45972" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{1722F03E-A338-4BDB-920F-BA87EA8992B5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16795" uniqueCount="16589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16863" uniqueCount="16594">
   <si>
     <t>Date</t>
   </si>
@@ -49803,6 +49803,21 @@
   </si>
   <si>
     <t>c5a637af-8aa7-42ee-b8e8-9ba48a3337dd</t>
+  </si>
+  <si>
+    <t>92488650-0c81-4876-a646-59747c1257da</t>
+  </si>
+  <si>
+    <t>Custom 2 Triggered</t>
+  </si>
+  <si>
+    <t>718e67c5-ccc9-4887-ac69-6a16954cbdfc</t>
+  </si>
+  <si>
+    <t>f6db5a71-4dc9-4176-b0bb-e23dd9818dab</t>
+  </si>
+  <si>
+    <t>5e513e39-eeaf-4424-b40a-1c2ac031f8f4</t>
   </si>
 </sst>
 </file>
@@ -50287,11 +50302,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E3A69F-5804-46B3-8092-81B33E8A06FF}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:XFD88"/>
+  <dimension ref="A1:XFD106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C74" sqref="C74:D74"/>
+      <selection pane="bottomLeft" activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -101967,6 +101982,570 @@
         <v>16588</v>
       </c>
     </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A89" s="24">
+        <v>45816</v>
+      </c>
+      <c r="B89" s="2">
+        <v>0.60671296296296295</v>
+      </c>
+      <c r="C89">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D89">
+        <v>-0.06</v>
+      </c>
+      <c r="F89" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M89" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N89" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O89">
+        <v>325419.44</v>
+      </c>
+      <c r="P89">
+        <v>6031442.8799999999</v>
+      </c>
+      <c r="Q89" s="19" t="s">
+        <v>16589</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="31">
+        <v>45816</v>
+      </c>
+      <c r="B90" s="15">
+        <v>0.60675925925925922</v>
+      </c>
+      <c r="C90" s="16">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D90" s="16">
+        <v>-0.06</v>
+      </c>
+      <c r="F90" s="16" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M90" s="16" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N90" s="16" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O90" s="16">
+        <v>325419.44</v>
+      </c>
+      <c r="P90" s="16">
+        <v>6031442.8799999999</v>
+      </c>
+      <c r="Q90" s="35" t="s">
+        <v>16591</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="31">
+        <v>45816</v>
+      </c>
+      <c r="B91" s="15">
+        <v>0.6069444444444444</v>
+      </c>
+      <c r="C91" s="16">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D91" s="16">
+        <v>-0.06</v>
+      </c>
+      <c r="F91" s="16" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M91" s="16" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N91" s="16" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O91" s="16">
+        <v>325419.44</v>
+      </c>
+      <c r="P91" s="16">
+        <v>6031442.8799999999</v>
+      </c>
+      <c r="Q91" s="35" t="s">
+        <v>16592</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="31">
+        <v>45816</v>
+      </c>
+      <c r="B92" s="15">
+        <v>0.60697916666666663</v>
+      </c>
+      <c r="C92" s="16">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D92" s="16">
+        <v>-0.06</v>
+      </c>
+      <c r="F92" s="16" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M92" s="16" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N92" s="16" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O92" s="16">
+        <v>325419.44</v>
+      </c>
+      <c r="P92" s="16">
+        <v>6031442.8799999999</v>
+      </c>
+      <c r="Q92" s="35" t="s">
+        <v>16593</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A93" s="24">
+        <v>45816</v>
+      </c>
+      <c r="B93" s="2">
+        <v>0.61518518518518517</v>
+      </c>
+      <c r="C93">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D93">
+        <v>-0.06</v>
+      </c>
+      <c r="F93" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M93" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N93" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O93">
+        <v>325419.44</v>
+      </c>
+      <c r="P93">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="31">
+        <v>45816</v>
+      </c>
+      <c r="B94" s="15">
+        <v>0.61524305555555558</v>
+      </c>
+      <c r="C94" s="16">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D94" s="16">
+        <v>-0.06</v>
+      </c>
+      <c r="F94" s="16" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M94" s="16" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N94" s="16" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O94" s="16">
+        <v>325419.44</v>
+      </c>
+      <c r="P94" s="16">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="26">
+        <v>45816</v>
+      </c>
+      <c r="B95" s="5">
+        <v>0.62124999999999997</v>
+      </c>
+      <c r="C95" s="6">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D95" s="6">
+        <v>-0.06</v>
+      </c>
+      <c r="F95" s="6" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M95" s="6" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N95" s="6" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O95" s="6">
+        <v>325419.44</v>
+      </c>
+      <c r="P95" s="6">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A96" s="24">
+        <v>45816</v>
+      </c>
+      <c r="B96" s="2">
+        <v>0.62127314814814816</v>
+      </c>
+      <c r="C96">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D96">
+        <v>-0.06</v>
+      </c>
+      <c r="F96" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M96" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N96" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O96">
+        <v>325419.44</v>
+      </c>
+      <c r="P96">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A97" s="24">
+        <v>45816</v>
+      </c>
+      <c r="B97" s="2">
+        <v>0.62230324074074073</v>
+      </c>
+      <c r="C97">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D97">
+        <v>-0.06</v>
+      </c>
+      <c r="E97" t="s">
+        <v>16567</v>
+      </c>
+      <c r="F97" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M97" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N97" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O97">
+        <v>325419.44</v>
+      </c>
+      <c r="P97">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="31">
+        <v>45816</v>
+      </c>
+      <c r="B98" s="15">
+        <v>0.62236111111111114</v>
+      </c>
+      <c r="C98" s="16">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D98" s="16">
+        <v>-0.06</v>
+      </c>
+      <c r="E98" s="16" t="s">
+        <v>16590</v>
+      </c>
+      <c r="F98" s="16" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M98" s="16" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N98" s="16" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O98" s="16">
+        <v>325419.44</v>
+      </c>
+      <c r="P98" s="16">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="26">
+        <v>45816</v>
+      </c>
+      <c r="B99" s="5">
+        <v>0.62239583333333337</v>
+      </c>
+      <c r="C99" s="6">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D99" s="6">
+        <v>-0.06</v>
+      </c>
+      <c r="E99" s="6" t="s">
+        <v>16383</v>
+      </c>
+      <c r="F99" s="6" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M99" s="6" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N99" s="6" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O99" s="6">
+        <v>325419.44</v>
+      </c>
+      <c r="P99" s="6">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="29">
+        <v>45817</v>
+      </c>
+      <c r="B100" s="11">
+        <v>1.1574074074074073E-5</v>
+      </c>
+      <c r="C100" s="12">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D100" s="12">
+        <v>-0.06</v>
+      </c>
+      <c r="E100" s="12" t="s">
+        <v>16387</v>
+      </c>
+      <c r="F100" s="12" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M100" s="12" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N100" s="12" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O100" s="12">
+        <v>325419.44</v>
+      </c>
+      <c r="P100" s="12">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="31">
+        <v>45817</v>
+      </c>
+      <c r="B101" s="15">
+        <v>0.17445601851851852</v>
+      </c>
+      <c r="C101" s="16">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D101" s="16">
+        <v>-0.06</v>
+      </c>
+      <c r="E101" s="16" t="s">
+        <v>16590</v>
+      </c>
+      <c r="F101" s="16" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M101" s="16" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N101" s="16" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O101" s="16">
+        <v>325419.44</v>
+      </c>
+      <c r="P101" s="16">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A102" s="24">
+        <v>45817</v>
+      </c>
+      <c r="B102" s="2">
+        <v>0.20101851851851851</v>
+      </c>
+      <c r="C102">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D102">
+        <v>-0.06</v>
+      </c>
+      <c r="E102" t="s">
+        <v>16567</v>
+      </c>
+      <c r="F102" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M102" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N102" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O102">
+        <v>325419.44</v>
+      </c>
+      <c r="P102">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="31">
+        <v>45817</v>
+      </c>
+      <c r="B103" s="15">
+        <v>0.2013425925925926</v>
+      </c>
+      <c r="C103" s="16">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D103" s="16">
+        <v>-0.06</v>
+      </c>
+      <c r="E103" s="16" t="s">
+        <v>16590</v>
+      </c>
+      <c r="F103" s="16" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M103" s="16" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N103" s="16" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O103" s="16">
+        <v>325419.44</v>
+      </c>
+      <c r="P103" s="16">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="31">
+        <v>45817</v>
+      </c>
+      <c r="B104" s="15">
+        <v>0.20199074074074075</v>
+      </c>
+      <c r="C104" s="16">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D104" s="16">
+        <v>-0.06</v>
+      </c>
+      <c r="E104" s="16" t="s">
+        <v>16590</v>
+      </c>
+      <c r="F104" s="16" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M104" s="16" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N104" s="16" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O104" s="16">
+        <v>325419.44</v>
+      </c>
+      <c r="P104" s="16">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="31">
+        <v>45817</v>
+      </c>
+      <c r="B105" s="15">
+        <v>0.20386574074074074</v>
+      </c>
+      <c r="C105" s="16">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D105" s="16">
+        <v>-0.06</v>
+      </c>
+      <c r="E105" s="16" t="s">
+        <v>16590</v>
+      </c>
+      <c r="F105" s="16" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M105" s="16" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N105" s="16" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O105" s="16">
+        <v>325419.44</v>
+      </c>
+      <c r="P105" s="16">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A106" s="24">
+        <v>45817</v>
+      </c>
+      <c r="B106" s="2">
+        <v>0.2038888888888889</v>
+      </c>
+      <c r="C106">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D106">
+        <v>-0.06</v>
+      </c>
+      <c r="E106" t="s">
+        <v>16567</v>
+      </c>
+      <c r="F106" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M106" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N106" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O106">
+        <v>325419.44</v>
+      </c>
+      <c r="P106">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- Updates to the Worker thread to accomodate the new custom button configuration - changes made in the create main buttons definition - errors where static text was not being written to the excel sheet - greater debugging
</commit_message>
<xml_diff>
--- a/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
+++ b/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\PYTHON\Online-Log-Development\Excel TEmplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C88608B-B675-450F-88ED-BD25692C1272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2F3D79-C0E5-400D-934D-7101C7E49129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45972" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{1722F03E-A338-4BDB-920F-BA87EA8992B5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16863" uniqueCount="16594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16900" uniqueCount="16595">
   <si>
     <t>Date</t>
   </si>
@@ -49818,6 +49818,9 @@
   </si>
   <si>
     <t>5e513e39-eeaf-4424-b40a-1c2ac031f8f4</t>
+  </si>
+  <si>
+    <t>Custom 4 Event</t>
   </si>
 </sst>
 </file>
@@ -50302,10 +50305,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E3A69F-5804-46B3-8092-81B33E8A06FF}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:XFD106"/>
+  <dimension ref="A1:XFD116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
@@ -102546,6 +102549,317 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
+    <row r="107" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="31">
+        <v>45817</v>
+      </c>
+      <c r="B107" s="15">
+        <v>0.20533564814814814</v>
+      </c>
+      <c r="C107" s="16">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D107" s="16">
+        <v>-0.06</v>
+      </c>
+      <c r="E107" s="16" t="s">
+        <v>16590</v>
+      </c>
+      <c r="F107" s="16" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M107" s="16" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N107" s="16" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O107" s="16">
+        <v>325419.44</v>
+      </c>
+      <c r="P107" s="16">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="29">
+        <v>45817</v>
+      </c>
+      <c r="B108" s="11">
+        <v>0.20600694444444445</v>
+      </c>
+      <c r="C108" s="12">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D108" s="12">
+        <v>-0.06</v>
+      </c>
+      <c r="E108" s="12" t="s">
+        <v>16387</v>
+      </c>
+      <c r="F108" s="12" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M108" s="12" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N108" s="12" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O108" s="12">
+        <v>325419.44</v>
+      </c>
+      <c r="P108" s="12">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A109" s="24">
+        <v>45817</v>
+      </c>
+      <c r="B109" s="2">
+        <v>0.20605324074074075</v>
+      </c>
+      <c r="C109">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D109">
+        <v>-0.06</v>
+      </c>
+      <c r="E109" t="s">
+        <v>16594</v>
+      </c>
+      <c r="F109" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M109" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N109" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O109">
+        <v>325419.44</v>
+      </c>
+      <c r="P109">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="31">
+        <v>45817</v>
+      </c>
+      <c r="B110" s="15">
+        <v>0.20668981481481483</v>
+      </c>
+      <c r="C110" s="16">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D110" s="16">
+        <v>-0.06</v>
+      </c>
+      <c r="E110" s="16" t="s">
+        <v>16590</v>
+      </c>
+      <c r="F110" s="16" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M110" s="16" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N110" s="16" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O110" s="16">
+        <v>325419.44</v>
+      </c>
+      <c r="P110" s="16">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A111" s="24">
+        <v>45817</v>
+      </c>
+      <c r="B111" s="2">
+        <v>0.21518518518518517</v>
+      </c>
+      <c r="C111">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D111">
+        <v>-0.06</v>
+      </c>
+      <c r="F111" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M111" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N111" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O111">
+        <v>325419.44</v>
+      </c>
+      <c r="P111">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="31">
+        <v>45817</v>
+      </c>
+      <c r="B112" s="15">
+        <v>0.21525462962962963</v>
+      </c>
+      <c r="C112" s="16">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D112" s="16">
+        <v>-0.06</v>
+      </c>
+      <c r="F112" s="16" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M112" s="16" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N112" s="16" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O112" s="16">
+        <v>325419.44</v>
+      </c>
+      <c r="P112" s="16">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="26">
+        <v>45817</v>
+      </c>
+      <c r="B113" s="5">
+        <v>0.21530092592592592</v>
+      </c>
+      <c r="C113" s="6">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D113" s="6">
+        <v>-0.06</v>
+      </c>
+      <c r="F113" s="6" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M113" s="6" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N113" s="6" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O113" s="6">
+        <v>325419.44</v>
+      </c>
+      <c r="P113" s="6">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A114" s="24">
+        <v>45817</v>
+      </c>
+      <c r="B114" s="2">
+        <v>0.21686342592592592</v>
+      </c>
+      <c r="C114">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D114">
+        <v>-0.06</v>
+      </c>
+      <c r="E114" t="s">
+        <v>16567</v>
+      </c>
+      <c r="F114" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M114" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N114" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O114">
+        <v>325419.44</v>
+      </c>
+      <c r="P114">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="26">
+        <v>45817</v>
+      </c>
+      <c r="B115" s="5">
+        <v>0.21726851851851853</v>
+      </c>
+      <c r="C115" s="6">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D115" s="6">
+        <v>-0.06</v>
+      </c>
+      <c r="E115" s="6" t="s">
+        <v>16383</v>
+      </c>
+      <c r="F115" s="6" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M115" s="6" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N115" s="6" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O115" s="6">
+        <v>325419.44</v>
+      </c>
+      <c r="P115" s="6">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A116" s="24">
+        <v>45817</v>
+      </c>
+      <c r="B116" s="2">
+        <v>0.21729166666666666</v>
+      </c>
+      <c r="C116">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D116">
+        <v>-0.06</v>
+      </c>
+      <c r="E116" t="s">
+        <v>16567</v>
+      </c>
+      <c r="F116" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M116" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N116" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O116">
+        <v>325419.44</v>
+      </c>
+      <c r="P116">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
-Tab creation function now handled with a right click -Layout now allows 5 buttons in a line before starting the next row -User can now rename the tabs and delete them where required
</commit_message>
<xml_diff>
--- a/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
+++ b/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\PYTHON\Online-Log-Development\Excel TEmplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2F3D79-C0E5-400D-934D-7101C7E49129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EE1762-3AD2-4E8B-9CCF-F3C3605415C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45972" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{1722F03E-A338-4BDB-920F-BA87EA8992B5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16900" uniqueCount="16595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16904" uniqueCount="16596">
   <si>
     <t>Date</t>
   </si>
@@ -49821,6 +49821,9 @@
   </si>
   <si>
     <t>Custom 4 Event</t>
+  </si>
+  <si>
+    <t>Custom 11 Event</t>
   </si>
 </sst>
 </file>
@@ -50305,11 +50308,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E3A69F-5804-46B3-8092-81B33E8A06FF}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:XFD116"/>
+  <dimension ref="A1:XFD117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E95" sqref="E95"/>
+      <selection pane="bottomLeft" activeCell="E117" sqref="E117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -102860,6 +102863,38 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
+    <row r="117" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A117" s="24">
+        <v>45817</v>
+      </c>
+      <c r="B117" s="2">
+        <v>0.31699074074074074</v>
+      </c>
+      <c r="C117">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D117">
+        <v>-0.06</v>
+      </c>
+      <c r="E117" t="s">
+        <v>16595</v>
+      </c>
+      <c r="F117" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M117" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N117" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O117">
+        <v>325419.44</v>
+      </c>
+      <c r="P117">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- Updated NExt steps
</commit_message>
<xml_diff>
--- a/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
+++ b/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\PYTHON\Online-Log-Development\Excel TEmplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EE1762-3AD2-4E8B-9CCF-F3C3605415C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB5C330-9046-4775-8B3D-7753B656E9AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45972" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{1722F03E-A338-4BDB-920F-BA87EA8992B5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16904" uniqueCount="16596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16997" uniqueCount="16642">
   <si>
     <t>Date</t>
   </si>
@@ -49824,6 +49824,144 @@
   </si>
   <si>
     <t>Custom 11 Event</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>273_REV05_20240605</t>
+  </si>
+  <si>
+    <t>54;24;03.01866N</t>
+  </si>
+  <si>
+    <t>12;18;37.03577E</t>
+  </si>
+  <si>
+    <t>54;24;03.01399N</t>
+  </si>
+  <si>
+    <t>12;18;37.03365E</t>
+  </si>
+  <si>
+    <t>Custom Event 2 Triggered</t>
+  </si>
+  <si>
+    <t>Custom Event 3 Triggered</t>
+  </si>
+  <si>
+    <t>54;24;03.01489N</t>
+  </si>
+  <si>
+    <t>12;18;37.03878E</t>
+  </si>
+  <si>
+    <t>Custom Event 1 Triggered</t>
+  </si>
+  <si>
+    <t>54;24;03.01519N</t>
+  </si>
+  <si>
+    <t>12;18;37.03969E</t>
+  </si>
+  <si>
+    <t>54;24;03.01670N</t>
+  </si>
+  <si>
+    <t>12;18;37.04301E</t>
+  </si>
+  <si>
+    <t>41;41;12.05519N</t>
+  </si>
+  <si>
+    <t>8;49;45.00442W</t>
+  </si>
+  <si>
+    <t>54;24;03.03722N</t>
+  </si>
+  <si>
+    <t>12;18;37.05719E</t>
+  </si>
+  <si>
+    <t>54;24;03.05005N</t>
+  </si>
+  <si>
+    <t>12;18;37.07107E</t>
+  </si>
+  <si>
+    <t>54;24;03.05020N</t>
+  </si>
+  <si>
+    <t>12;18;37.07167E</t>
+  </si>
+  <si>
+    <t>12;18;37.07137E</t>
+  </si>
+  <si>
+    <t>54;24;03.05035N</t>
+  </si>
+  <si>
+    <t>12;18;37.07047E</t>
+  </si>
+  <si>
+    <t>54;24;03.05065N</t>
+  </si>
+  <si>
+    <t>12;18;37.06836E</t>
+  </si>
+  <si>
+    <t>54;24;03.05050N</t>
+  </si>
+  <si>
+    <t>12;18;37.06805E</t>
+  </si>
+  <si>
+    <t>54;24;03.07403N</t>
+  </si>
+  <si>
+    <t>12;18;36.91175E</t>
+  </si>
+  <si>
+    <t>54;24;03.07388N</t>
+  </si>
+  <si>
+    <t>12;18;36.91145E</t>
+  </si>
+  <si>
+    <t>54;24;03.07449N</t>
+  </si>
+  <si>
+    <t>12;18;36.91205E</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>54;24;03.10029N</t>
+  </si>
+  <si>
+    <t>12;18;36.35502E</t>
+  </si>
+  <si>
+    <t>54;24;03.10044N</t>
+  </si>
+  <si>
+    <t>12;18;36.35532E</t>
+  </si>
+  <si>
+    <t>Custom 6 Event</t>
+  </si>
+  <si>
+    <t>54;24;03.10089N</t>
+  </si>
+  <si>
+    <t>12;18;36.35653E</t>
+  </si>
+  <si>
+    <t>54;24;03.10134N</t>
+  </si>
+  <si>
+    <t>12;18;36.35683E</t>
   </si>
 </sst>
 </file>
@@ -50308,11 +50446,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E3A69F-5804-46B3-8092-81B33E8A06FF}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:XFD117"/>
+  <dimension ref="A1:XFD142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E117" sqref="E117"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E143" sqref="E143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -102895,6 +103033,770 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
+    <row r="118" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="28">
+        <v>45817</v>
+      </c>
+      <c r="B118" s="9">
+        <v>0.51842592592592596</v>
+      </c>
+      <c r="C118" s="10">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D118" s="10">
+        <v>-0.06</v>
+      </c>
+      <c r="F118" s="10" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M118" s="10" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N118" s="10" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O118" s="10">
+        <v>325419.44</v>
+      </c>
+      <c r="P118" s="10">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="31">
+        <v>45817</v>
+      </c>
+      <c r="B119" s="15">
+        <v>0.5188194444444445</v>
+      </c>
+      <c r="C119" s="16">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D119" s="16">
+        <v>-0.06</v>
+      </c>
+      <c r="E119" s="16" t="s">
+        <v>16596</v>
+      </c>
+      <c r="F119" s="16" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M119" s="16" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N119" s="16" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O119" s="16">
+        <v>325419.44</v>
+      </c>
+      <c r="P119" s="16">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="31">
+        <v>45817</v>
+      </c>
+      <c r="B120" s="15">
+        <v>0.51885416666666662</v>
+      </c>
+      <c r="C120" s="16">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D120" s="16">
+        <v>-0.06</v>
+      </c>
+      <c r="E120" s="16" t="s">
+        <v>16596</v>
+      </c>
+      <c r="F120" s="16" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M120" s="16" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N120" s="16" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O120" s="16">
+        <v>325419.44</v>
+      </c>
+      <c r="P120" s="16">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="26">
+        <v>45817</v>
+      </c>
+      <c r="B121" s="5">
+        <v>0.55883101851851846</v>
+      </c>
+      <c r="C121" s="6">
+        <v>15.952999999999999</v>
+      </c>
+      <c r="D121" s="6">
+        <v>-36.18</v>
+      </c>
+      <c r="E121" s="6" t="s">
+        <v>16383</v>
+      </c>
+      <c r="F121" s="6" t="s">
+        <v>16597</v>
+      </c>
+      <c r="M121" s="6" t="s">
+        <v>16598</v>
+      </c>
+      <c r="N121" s="6" t="s">
+        <v>16599</v>
+      </c>
+      <c r="O121" s="6">
+        <v>325409.33</v>
+      </c>
+      <c r="P121" s="6">
+        <v>6031453.8099999996</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="28">
+        <v>45817</v>
+      </c>
+      <c r="B122" s="9">
+        <v>0.55905092592592598</v>
+      </c>
+      <c r="C122" s="10">
+        <v>15.952999999999999</v>
+      </c>
+      <c r="D122" s="10">
+        <v>-36.24</v>
+      </c>
+      <c r="F122" s="10" t="s">
+        <v>16597</v>
+      </c>
+      <c r="M122" s="10" t="s">
+        <v>16600</v>
+      </c>
+      <c r="N122" s="10" t="s">
+        <v>16601</v>
+      </c>
+      <c r="O122" s="10">
+        <v>325409.28999999998</v>
+      </c>
+      <c r="P122" s="10">
+        <v>6031453.6699999999</v>
+      </c>
+    </row>
+    <row r="123" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A123" s="24">
+        <v>45817</v>
+      </c>
+      <c r="B123" s="2">
+        <v>0.5591666666666667</v>
+      </c>
+      <c r="C123">
+        <v>15.952999999999999</v>
+      </c>
+      <c r="D123">
+        <v>-36.29</v>
+      </c>
+      <c r="E123" t="s">
+        <v>16606</v>
+      </c>
+      <c r="F123" t="s">
+        <v>16597</v>
+      </c>
+      <c r="M123" t="s">
+        <v>16604</v>
+      </c>
+      <c r="N123" t="s">
+        <v>16605</v>
+      </c>
+      <c r="O123">
+        <v>325409.38</v>
+      </c>
+      <c r="P123">
+        <v>6031453.6900000004</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A124" s="24">
+        <v>45817</v>
+      </c>
+      <c r="B124" s="2">
+        <v>0.55920138888888893</v>
+      </c>
+      <c r="C124">
+        <v>15.952999999999999</v>
+      </c>
+      <c r="D124">
+        <v>-36.299999999999997</v>
+      </c>
+      <c r="E124" t="s">
+        <v>16606</v>
+      </c>
+      <c r="F124" t="s">
+        <v>16597</v>
+      </c>
+      <c r="M124" t="s">
+        <v>16607</v>
+      </c>
+      <c r="N124" t="s">
+        <v>16608</v>
+      </c>
+      <c r="O124">
+        <v>325409.40000000002</v>
+      </c>
+      <c r="P124">
+        <v>6031453.7000000002</v>
+      </c>
+    </row>
+    <row r="125" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A125" s="24">
+        <v>45817</v>
+      </c>
+      <c r="B125" s="2">
+        <v>0.55935185185185188</v>
+      </c>
+      <c r="C125">
+        <v>15.952999999999999</v>
+      </c>
+      <c r="D125">
+        <v>-36.32</v>
+      </c>
+      <c r="E125" t="s">
+        <v>16602</v>
+      </c>
+      <c r="F125" t="s">
+        <v>16597</v>
+      </c>
+      <c r="M125" t="s">
+        <v>16609</v>
+      </c>
+      <c r="N125" t="s">
+        <v>16610</v>
+      </c>
+      <c r="O125">
+        <v>325409.46000000002</v>
+      </c>
+      <c r="P125">
+        <v>6031453.75</v>
+      </c>
+    </row>
+    <row r="126" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A126" s="24">
+        <v>45817</v>
+      </c>
+      <c r="B126" s="2">
+        <v>0.56067129629629631</v>
+      </c>
+      <c r="E126" t="s">
+        <v>16606</v>
+      </c>
+      <c r="M126" t="s">
+        <v>16611</v>
+      </c>
+      <c r="N126" t="s">
+        <v>16612</v>
+      </c>
+      <c r="O126">
+        <v>514217.1</v>
+      </c>
+      <c r="P126">
+        <v>4615003.93</v>
+      </c>
+    </row>
+    <row r="127" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A127" s="24">
+        <v>45817</v>
+      </c>
+      <c r="B127" s="2">
+        <v>0.56098379629629624</v>
+      </c>
+      <c r="C127">
+        <v>15.952999999999999</v>
+      </c>
+      <c r="E127" t="s">
+        <v>16602</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A128" s="24">
+        <v>45817</v>
+      </c>
+      <c r="B128" s="2">
+        <v>0.56128472222222225</v>
+      </c>
+      <c r="C128">
+        <v>15.952999999999999</v>
+      </c>
+      <c r="D128">
+        <v>-36.15</v>
+      </c>
+      <c r="E128" t="s">
+        <v>16606</v>
+      </c>
+      <c r="F128" t="s">
+        <v>16597</v>
+      </c>
+      <c r="M128" t="s">
+        <v>16613</v>
+      </c>
+      <c r="N128" t="s">
+        <v>16614</v>
+      </c>
+      <c r="O128">
+        <v>325409.74</v>
+      </c>
+      <c r="P128">
+        <v>6031454.3700000001</v>
+      </c>
+    </row>
+    <row r="129" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A129" s="24">
+        <v>45817</v>
+      </c>
+      <c r="B129" s="2">
+        <v>0.56146990740740743</v>
+      </c>
+      <c r="C129">
+        <v>15.954000000000001</v>
+      </c>
+      <c r="D129">
+        <v>-36.119999999999997</v>
+      </c>
+      <c r="E129" t="s">
+        <v>16603</v>
+      </c>
+      <c r="F129" t="s">
+        <v>16597</v>
+      </c>
+      <c r="M129" t="s">
+        <v>16615</v>
+      </c>
+      <c r="N129" t="s">
+        <v>16616</v>
+      </c>
+      <c r="O129">
+        <v>325410.01</v>
+      </c>
+      <c r="P129">
+        <v>6031454.7599999998</v>
+      </c>
+    </row>
+    <row r="130" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A130" s="24">
+        <v>45817</v>
+      </c>
+      <c r="B130" s="2">
+        <v>0.56149305555555551</v>
+      </c>
+      <c r="C130">
+        <v>15.954000000000001</v>
+      </c>
+      <c r="D130">
+        <v>-36.119999999999997</v>
+      </c>
+      <c r="E130" t="s">
+        <v>16602</v>
+      </c>
+      <c r="F130" t="s">
+        <v>16597</v>
+      </c>
+      <c r="M130" t="s">
+        <v>16617</v>
+      </c>
+      <c r="N130" t="s">
+        <v>16618</v>
+      </c>
+      <c r="O130">
+        <v>325410.02</v>
+      </c>
+      <c r="P130">
+        <v>6031454.7599999998</v>
+      </c>
+    </row>
+    <row r="131" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="26">
+        <v>45817</v>
+      </c>
+      <c r="B131" s="5">
+        <v>0.5615162037037037</v>
+      </c>
+      <c r="C131" s="6">
+        <v>15.954000000000001</v>
+      </c>
+      <c r="D131" s="6">
+        <v>-36.119999999999997</v>
+      </c>
+      <c r="E131" s="6" t="s">
+        <v>16383</v>
+      </c>
+      <c r="F131" s="6" t="s">
+        <v>16597</v>
+      </c>
+      <c r="M131" s="6" t="s">
+        <v>16617</v>
+      </c>
+      <c r="N131" s="6" t="s">
+        <v>16619</v>
+      </c>
+      <c r="O131" s="6">
+        <v>325410.01</v>
+      </c>
+      <c r="P131" s="6">
+        <v>6031454.7599999998</v>
+      </c>
+    </row>
+    <row r="132" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="28">
+        <v>45817</v>
+      </c>
+      <c r="B132" s="9">
+        <v>0.56155092592592593</v>
+      </c>
+      <c r="C132" s="10">
+        <v>15.954000000000001</v>
+      </c>
+      <c r="D132" s="10">
+        <v>-36.1</v>
+      </c>
+      <c r="F132" s="10" t="s">
+        <v>16597</v>
+      </c>
+      <c r="M132" s="10" t="s">
+        <v>16620</v>
+      </c>
+      <c r="N132" s="10" t="s">
+        <v>16621</v>
+      </c>
+      <c r="O132" s="10">
+        <v>325410</v>
+      </c>
+      <c r="P132" s="10">
+        <v>6031454.7699999996</v>
+      </c>
+    </row>
+    <row r="133" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="27">
+        <v>45817</v>
+      </c>
+      <c r="B133" s="7">
+        <v>0.56160879629629634</v>
+      </c>
+      <c r="C133" s="8">
+        <v>15.954000000000001</v>
+      </c>
+      <c r="D133" s="8">
+        <v>-36.07</v>
+      </c>
+      <c r="E133" s="8" t="s">
+        <v>16384</v>
+      </c>
+      <c r="F133" s="8" t="s">
+        <v>16597</v>
+      </c>
+      <c r="M133" s="8" t="s">
+        <v>16622</v>
+      </c>
+      <c r="N133" s="8" t="s">
+        <v>16623</v>
+      </c>
+      <c r="O133" s="8">
+        <v>325409.96000000002</v>
+      </c>
+      <c r="P133" s="8">
+        <v>6031454.7800000003</v>
+      </c>
+    </row>
+    <row r="134" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="29">
+        <v>45817</v>
+      </c>
+      <c r="B134" s="11">
+        <v>0.56164351851851857</v>
+      </c>
+      <c r="C134" s="12">
+        <v>15.954000000000001</v>
+      </c>
+      <c r="D134" s="12">
+        <v>-36.07</v>
+      </c>
+      <c r="E134" s="12" t="s">
+        <v>16387</v>
+      </c>
+      <c r="F134" s="12" t="s">
+        <v>16597</v>
+      </c>
+      <c r="M134" s="12" t="s">
+        <v>16624</v>
+      </c>
+      <c r="N134" s="12" t="s">
+        <v>16625</v>
+      </c>
+      <c r="O134" s="12">
+        <v>325409.95</v>
+      </c>
+      <c r="P134" s="12">
+        <v>6031454.7699999996</v>
+      </c>
+    </row>
+    <row r="135" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A135" s="24">
+        <v>45817</v>
+      </c>
+      <c r="B135" s="2">
+        <v>0.56910879629629629</v>
+      </c>
+      <c r="C135">
+        <v>15.952999999999999</v>
+      </c>
+      <c r="D135">
+        <v>-33.36</v>
+      </c>
+      <c r="E135" t="s">
+        <v>16606</v>
+      </c>
+      <c r="F135" t="s">
+        <v>16597</v>
+      </c>
+      <c r="M135" t="s">
+        <v>16626</v>
+      </c>
+      <c r="N135" t="s">
+        <v>16627</v>
+      </c>
+      <c r="O135">
+        <v>325407.15999999997</v>
+      </c>
+      <c r="P135">
+        <v>6031455.6100000003</v>
+      </c>
+    </row>
+    <row r="136" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A136" s="24">
+        <v>45817</v>
+      </c>
+      <c r="B136" s="2">
+        <v>0.56913194444444448</v>
+      </c>
+      <c r="C136">
+        <v>15.952999999999999</v>
+      </c>
+      <c r="D136">
+        <v>-33.36</v>
+      </c>
+      <c r="E136" t="s">
+        <v>16602</v>
+      </c>
+      <c r="F136" t="s">
+        <v>16597</v>
+      </c>
+      <c r="M136" t="s">
+        <v>16626</v>
+      </c>
+      <c r="N136" t="s">
+        <v>16627</v>
+      </c>
+      <c r="O136">
+        <v>325407.15999999997</v>
+      </c>
+      <c r="P136">
+        <v>6031455.6100000003</v>
+      </c>
+    </row>
+    <row r="137" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="26">
+        <v>45817</v>
+      </c>
+      <c r="B137" s="5">
+        <v>0.56916666666666671</v>
+      </c>
+      <c r="C137" s="6">
+        <v>15.952999999999999</v>
+      </c>
+      <c r="D137" s="6">
+        <v>-33.36</v>
+      </c>
+      <c r="E137" s="6" t="s">
+        <v>16383</v>
+      </c>
+      <c r="F137" s="6" t="s">
+        <v>16597</v>
+      </c>
+      <c r="M137" s="6" t="s">
+        <v>16628</v>
+      </c>
+      <c r="N137" s="6" t="s">
+        <v>16629</v>
+      </c>
+      <c r="O137" s="6">
+        <v>325407.15999999997</v>
+      </c>
+      <c r="P137" s="6">
+        <v>6031455.5999999996</v>
+      </c>
+    </row>
+    <row r="138" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="31">
+        <v>45817</v>
+      </c>
+      <c r="B138" s="15">
+        <v>0.56945601851851857</v>
+      </c>
+      <c r="C138" s="16">
+        <v>15.952999999999999</v>
+      </c>
+      <c r="D138" s="16">
+        <v>-33.36</v>
+      </c>
+      <c r="E138" s="16" t="s">
+        <v>16632</v>
+      </c>
+      <c r="F138" s="16" t="s">
+        <v>16597</v>
+      </c>
+      <c r="M138" s="16" t="s">
+        <v>16630</v>
+      </c>
+      <c r="N138" s="16" t="s">
+        <v>16631</v>
+      </c>
+      <c r="O138" s="16">
+        <v>325407.17</v>
+      </c>
+      <c r="P138" s="16">
+        <v>6031455.6200000001</v>
+      </c>
+    </row>
+    <row r="139" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="26">
+        <v>45817</v>
+      </c>
+      <c r="B139" s="5">
+        <v>0.58832175925925922</v>
+      </c>
+      <c r="C139" s="6">
+        <v>15.948</v>
+      </c>
+      <c r="D139" s="6">
+        <v>-24.8</v>
+      </c>
+      <c r="E139" s="6" t="s">
+        <v>16383</v>
+      </c>
+      <c r="F139" s="6" t="s">
+        <v>16597</v>
+      </c>
+      <c r="M139" s="6" t="s">
+        <v>16633</v>
+      </c>
+      <c r="N139" s="6" t="s">
+        <v>16634</v>
+      </c>
+      <c r="O139" s="6">
+        <v>325397.15999999997</v>
+      </c>
+      <c r="P139" s="6">
+        <v>6031456.7999999998</v>
+      </c>
+    </row>
+    <row r="140" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A140" s="24">
+        <v>45817</v>
+      </c>
+      <c r="B140" s="2">
+        <v>0.58835648148148145</v>
+      </c>
+      <c r="C140">
+        <v>15.948</v>
+      </c>
+      <c r="D140">
+        <v>-24.8</v>
+      </c>
+      <c r="E140" t="s">
+        <v>16602</v>
+      </c>
+      <c r="F140" t="s">
+        <v>16597</v>
+      </c>
+      <c r="M140" t="s">
+        <v>16635</v>
+      </c>
+      <c r="N140" t="s">
+        <v>16636</v>
+      </c>
+      <c r="O140">
+        <v>325397.17</v>
+      </c>
+      <c r="P140">
+        <v>6031456.8099999996</v>
+      </c>
+    </row>
+    <row r="141" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A141" s="24">
+        <v>45817</v>
+      </c>
+      <c r="B141" s="2">
+        <v>0.58858796296296301</v>
+      </c>
+      <c r="C141">
+        <v>15.948</v>
+      </c>
+      <c r="D141">
+        <v>-24.81</v>
+      </c>
+      <c r="E141" t="s">
+        <v>16602</v>
+      </c>
+      <c r="F141" t="s">
+        <v>16597</v>
+      </c>
+      <c r="M141" t="s">
+        <v>16638</v>
+      </c>
+      <c r="N141" t="s">
+        <v>16639</v>
+      </c>
+      <c r="O141">
+        <v>325397.19</v>
+      </c>
+      <c r="P141">
+        <v>6031456.8200000003</v>
+      </c>
+    </row>
+    <row r="142" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A142" s="24">
+        <v>45817</v>
+      </c>
+      <c r="B142" s="2">
+        <v>0.58872685185185181</v>
+      </c>
+      <c r="C142">
+        <v>15.948</v>
+      </c>
+      <c r="D142">
+        <v>-24.8</v>
+      </c>
+      <c r="E142" t="s">
+        <v>16637</v>
+      </c>
+      <c r="F142" t="s">
+        <v>16597</v>
+      </c>
+      <c r="M142" t="s">
+        <v>16640</v>
+      </c>
+      <c r="N142" t="s">
+        <v>16641</v>
+      </c>
+      <c r="O142">
+        <v>325397.19</v>
+      </c>
+      <c r="P142">
+        <v>6031456.8300000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- KP hourly log automatic event added
- Programmed events tab added in the Settings menu enable or disable and define the color of the programmed events (Midnight new day and KP hourly)
</commit_message>
<xml_diff>
--- a/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
+++ b/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\PYTHON\Online-Log-Development\Excel TEmplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\PYTHON\Vicente\Online-Log-Development\Excel TEmplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB5C330-9046-4775-8B3D-7753B656E9AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E959CA7F-181A-430E-AEF0-74B1E825A5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{1722F03E-A338-4BDB-920F-BA87EA8992B5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{1722F03E-A338-4BDB-920F-BA87EA8992B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16997" uniqueCount="16642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17005" uniqueCount="16643">
   <si>
     <t>Date</t>
   </si>
@@ -49962,6 +49962,9 @@
   </si>
   <si>
     <t>12;18;36.35683E</t>
+  </si>
+  <si>
+    <t>Hourly KP Log</t>
   </si>
 </sst>
 </file>
@@ -49988,7 +49991,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -50055,6 +50058,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF80FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -50068,7 +50077,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -50111,6 +50120,9 @@
     <xf numFmtId="21" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="21" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -50446,24 +50458,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E3A69F-5804-46B3-8092-81B33E8A06FF}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:XFD142"/>
+  <dimension ref="A1:XFD294"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E143" sqref="E143"/>
+      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E144" sqref="E144"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.44140625" customWidth="1"/>
-    <col min="6" max="6" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="101.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.36328125" style="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.453125" customWidth="1"/>
+    <col min="6" max="6" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="101.81640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="38.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16384" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -99617,7 +99629,7 @@
         <v>16382</v>
       </c>
     </row>
-    <row r="2" spans="1:16384" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16384" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="32">
         <v>45774</v>
       </c>
@@ -99658,7 +99670,7 @@
         <v>16395</v>
       </c>
     </row>
-    <row r="3" spans="1:16384" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16384" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="29">
         <v>45774</v>
       </c>
@@ -99699,7 +99711,7 @@
         <v>16398</v>
       </c>
     </row>
-    <row r="4" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="28">
         <v>45774</v>
       </c>
@@ -99731,7 +99743,7 @@
         <v>16401</v>
       </c>
     </row>
-    <row r="5" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="28">
         <v>45774</v>
       </c>
@@ -99763,7 +99775,7 @@
         <v>16404</v>
       </c>
     </row>
-    <row r="6" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="28">
         <v>45774</v>
       </c>
@@ -99798,7 +99810,7 @@
         <v>16406</v>
       </c>
     </row>
-    <row r="7" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="28">
         <v>45774</v>
       </c>
@@ -99830,7 +99842,7 @@
         <v>16409</v>
       </c>
     </row>
-    <row r="8" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="28">
         <v>45774</v>
       </c>
@@ -99865,7 +99877,7 @@
         <v>16412</v>
       </c>
     </row>
-    <row r="9" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="28">
         <v>45774</v>
       </c>
@@ -99897,7 +99909,7 @@
         <v>16415</v>
       </c>
     </row>
-    <row r="10" spans="1:16384" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16384" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="32">
         <v>45774</v>
       </c>
@@ -99938,7 +99950,7 @@
         <v>16420</v>
       </c>
     </row>
-    <row r="11" spans="1:16384" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16384" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="32">
         <v>45774</v>
       </c>
@@ -99979,7 +99991,7 @@
         <v>16423</v>
       </c>
     </row>
-    <row r="12" spans="1:16384" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16384" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="25">
         <v>45774</v>
       </c>
@@ -100020,7 +100032,7 @@
         <v>16428</v>
       </c>
     </row>
-    <row r="13" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16384" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="28">
         <v>45774</v>
       </c>
@@ -100052,7 +100064,7 @@
         <v>16431</v>
       </c>
     </row>
-    <row r="14" spans="1:16384" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16384" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="25">
         <v>45774</v>
       </c>
@@ -100093,7 +100105,7 @@
         <v>16434</v>
       </c>
     </row>
-    <row r="15" spans="1:16384" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16384" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="29">
         <v>45774</v>
       </c>
@@ -100134,7 +100146,7 @@
         <v>16437</v>
       </c>
     </row>
-    <row r="16" spans="1:16384" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16384" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="30">
         <v>45774</v>
       </c>
@@ -100175,7 +100187,7 @@
         <v>16440</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="32">
         <v>45774</v>
       </c>
@@ -100216,7 +100228,7 @@
         <v>16444</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="25">
         <v>45774</v>
       </c>
@@ -100257,7 +100269,7 @@
         <v>16447</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="29">
         <v>45774</v>
       </c>
@@ -100298,7 +100310,7 @@
         <v>16450</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="32">
         <v>45774</v>
       </c>
@@ -100339,7 +100351,7 @@
         <v>16453</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="25">
         <v>45774</v>
       </c>
@@ -100380,7 +100392,7 @@
         <v>16456</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="30">
         <v>45774</v>
       </c>
@@ -100421,7 +100433,7 @@
         <v>16458</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="25">
         <v>45774</v>
       </c>
@@ -100462,7 +100474,7 @@
         <v>16461</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="29">
         <v>45774</v>
       </c>
@@ -100503,7 +100515,7 @@
         <v>16465</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="30">
         <v>45774</v>
       </c>
@@ -100544,7 +100556,7 @@
         <v>16469</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="31">
         <v>45774</v>
       </c>
@@ -100585,7 +100597,7 @@
         <v>16472</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="30">
         <v>45774</v>
       </c>
@@ -100626,7 +100638,7 @@
         <v>16475</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="26">
         <v>45775</v>
       </c>
@@ -100664,7 +100676,7 @@
         <v>16478</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="27">
         <v>45775</v>
       </c>
@@ -100702,7 +100714,7 @@
         <v>16483</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="24">
         <v>45775</v>
       </c>
@@ -100737,7 +100749,7 @@
         <v>16488</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="32">
         <v>45775</v>
       </c>
@@ -100778,7 +100790,7 @@
         <v>16492</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="25">
         <v>45775</v>
       </c>
@@ -100819,7 +100831,7 @@
         <v>16497</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="28">
         <v>45775</v>
       </c>
@@ -100851,7 +100863,7 @@
         <v>16501</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="30">
         <v>45775</v>
       </c>
@@ -100892,7 +100904,7 @@
         <v>16505</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="32">
         <v>45776</v>
       </c>
@@ -100913,7 +100925,7 @@
         <v>16509</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="25">
         <v>45776</v>
       </c>
@@ -100934,7 +100946,7 @@
         <v>16510</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="32">
         <v>45776</v>
       </c>
@@ -100955,7 +100967,7 @@
         <v>16511</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="32">
         <v>45776</v>
       </c>
@@ -100976,7 +100988,7 @@
         <v>16512</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="32">
         <v>45776</v>
       </c>
@@ -100999,7 +101011,7 @@
         <v>16513</v>
       </c>
     </row>
-    <row r="40" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="25">
         <v>45776</v>
       </c>
@@ -101022,7 +101034,7 @@
         <v>16514</v>
       </c>
     </row>
-    <row r="41" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="32">
         <v>45776</v>
       </c>
@@ -101045,7 +101057,7 @@
         <v>16515</v>
       </c>
     </row>
-    <row r="42" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="32">
         <v>45776</v>
       </c>
@@ -101068,7 +101080,7 @@
         <v>16516</v>
       </c>
     </row>
-    <row r="43" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="25">
         <v>45776</v>
       </c>
@@ -101091,7 +101103,7 @@
         <v>16517</v>
       </c>
     </row>
-    <row r="44" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="32">
         <v>45811</v>
       </c>
@@ -101114,7 +101126,7 @@
         <v>16518</v>
       </c>
     </row>
-    <row r="45" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="25">
         <v>45811</v>
       </c>
@@ -101137,7 +101149,7 @@
         <v>16521</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="24">
         <v>45811</v>
       </c>
@@ -101151,7 +101163,7 @@
         <v>16522</v>
       </c>
     </row>
-    <row r="47" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="30">
         <v>45811</v>
       </c>
@@ -101174,7 +101186,7 @@
         <v>16523</v>
       </c>
     </row>
-    <row r="48" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="29">
         <v>45812</v>
       </c>
@@ -101215,7 +101227,7 @@
         <v>16526</v>
       </c>
     </row>
-    <row r="49" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="29">
         <v>45812</v>
       </c>
@@ -101253,7 +101265,7 @@
         <v>16528</v>
       </c>
     </row>
-    <row r="50" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="32">
         <v>45812</v>
       </c>
@@ -101294,7 +101306,7 @@
         <v>16533</v>
       </c>
     </row>
-    <row r="51" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="25">
         <v>45812</v>
       </c>
@@ -101335,7 +101347,7 @@
         <v>16536</v>
       </c>
     </row>
-    <row r="52" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="30">
         <v>45812</v>
       </c>
@@ -101376,7 +101388,7 @@
         <v>16538</v>
       </c>
     </row>
-    <row r="53" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="30">
         <v>45812</v>
       </c>
@@ -101417,7 +101429,7 @@
         <v>16540</v>
       </c>
     </row>
-    <row r="54" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="31">
         <v>45812</v>
       </c>
@@ -101458,7 +101470,7 @@
         <v>16542</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="24">
         <v>45812</v>
       </c>
@@ -101499,7 +101511,7 @@
         <v>16544</v>
       </c>
     </row>
-    <row r="56" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="29">
         <v>45812</v>
       </c>
@@ -101540,7 +101552,7 @@
         <v>16547</v>
       </c>
     </row>
-    <row r="57" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="28">
         <v>45812</v>
       </c>
@@ -101572,7 +101584,7 @@
         <v>16549</v>
       </c>
     </row>
-    <row r="58" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="26">
         <v>45812</v>
       </c>
@@ -101586,7 +101598,7 @@
         <v>16552</v>
       </c>
     </row>
-    <row r="59" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="27">
         <v>45812</v>
       </c>
@@ -101600,7 +101612,7 @@
         <v>16553</v>
       </c>
     </row>
-    <row r="60" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="29">
         <v>45812</v>
       </c>
@@ -101614,7 +101626,7 @@
         <v>16554</v>
       </c>
     </row>
-    <row r="61" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="26">
         <v>45814</v>
       </c>
@@ -101628,7 +101640,7 @@
         <v>16555</v>
       </c>
     </row>
-    <row r="62" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="27">
         <v>45814</v>
       </c>
@@ -101642,7 +101654,7 @@
         <v>16556</v>
       </c>
     </row>
-    <row r="63" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="28">
         <v>45814</v>
       </c>
@@ -101653,7 +101665,7 @@
         <v>16557</v>
       </c>
     </row>
-    <row r="64" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="29">
         <v>45814</v>
       </c>
@@ -101667,7 +101679,7 @@
         <v>16558</v>
       </c>
     </row>
-    <row r="65" spans="1:17" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" s="40" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="38">
         <v>45814</v>
       </c>
@@ -101681,7 +101693,7 @@
         <v>16559</v>
       </c>
     </row>
-    <row r="66" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A66" s="29">
         <v>45815</v>
       </c>
@@ -101695,7 +101707,7 @@
         <v>16561</v>
       </c>
     </row>
-    <row r="67" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67" s="27">
         <v>45815</v>
       </c>
@@ -101709,7 +101721,7 @@
         <v>16562</v>
       </c>
     </row>
-    <row r="68" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68" s="26">
         <v>45815</v>
       </c>
@@ -101723,7 +101735,7 @@
         <v>16563</v>
       </c>
     </row>
-    <row r="69" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A69" s="27">
         <v>45815</v>
       </c>
@@ -101737,7 +101749,7 @@
         <v>16564</v>
       </c>
     </row>
-    <row r="70" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A70" s="28">
         <v>45815</v>
       </c>
@@ -101748,7 +101760,7 @@
         <v>16565</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" s="24">
         <v>45815</v>
       </c>
@@ -101765,7 +101777,7 @@
         <v>16566</v>
       </c>
     </row>
-    <row r="72" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A72" s="26">
         <v>45815</v>
       </c>
@@ -101782,7 +101794,7 @@
         <v>16569</v>
       </c>
     </row>
-    <row r="73" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A73" s="27">
         <v>45815</v>
       </c>
@@ -101799,7 +101811,7 @@
         <v>16570</v>
       </c>
     </row>
-    <row r="74" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A74" s="26">
         <v>45815</v>
       </c>
@@ -101813,7 +101825,7 @@
         <v>16571</v>
       </c>
     </row>
-    <row r="75" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A75" s="26">
         <v>45815</v>
       </c>
@@ -101827,7 +101839,7 @@
         <v>16572</v>
       </c>
     </row>
-    <row r="76" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A76" s="29">
         <v>45815</v>
       </c>
@@ -101841,7 +101853,7 @@
         <v>16573</v>
       </c>
     </row>
-    <row r="77" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A77" s="27">
         <v>45815</v>
       </c>
@@ -101855,7 +101867,7 @@
         <v>16574</v>
       </c>
     </row>
-    <row r="78" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A78" s="28">
         <v>45815</v>
       </c>
@@ -101866,7 +101878,7 @@
         <v>16575</v>
       </c>
     </row>
-    <row r="79" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A79" s="26">
         <v>45815</v>
       </c>
@@ -101880,7 +101892,7 @@
         <v>16576</v>
       </c>
     </row>
-    <row r="80" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A80" s="27">
         <v>45815</v>
       </c>
@@ -101894,7 +101906,7 @@
         <v>16577</v>
       </c>
     </row>
-    <row r="81" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A81" s="26">
         <v>45816</v>
       </c>
@@ -101908,7 +101920,7 @@
         <v>16578</v>
       </c>
     </row>
-    <row r="82" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A82" s="27">
         <v>45816</v>
       </c>
@@ -101922,7 +101934,7 @@
         <v>16579</v>
       </c>
     </row>
-    <row r="83" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A83" s="26">
         <v>45816</v>
       </c>
@@ -101957,7 +101969,7 @@
         <v>16580</v>
       </c>
     </row>
-    <row r="84" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A84" s="27">
         <v>45816</v>
       </c>
@@ -101992,7 +102004,7 @@
         <v>16584</v>
       </c>
     </row>
-    <row r="85" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A85" s="26">
         <v>45816</v>
       </c>
@@ -102027,7 +102039,7 @@
         <v>16585</v>
       </c>
     </row>
-    <row r="86" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A86" s="27">
         <v>45816</v>
       </c>
@@ -102062,7 +102074,7 @@
         <v>16586</v>
       </c>
     </row>
-    <row r="87" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A87" s="26">
         <v>45816</v>
       </c>
@@ -102094,7 +102106,7 @@
         <v>16587</v>
       </c>
     </row>
-    <row r="88" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A88" s="27">
         <v>45816</v>
       </c>
@@ -102126,7 +102138,7 @@
         <v>16588</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A89" s="24">
         <v>45816</v>
       </c>
@@ -102158,7 +102170,7 @@
         <v>16589</v>
       </c>
     </row>
-    <row r="90" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A90" s="31">
         <v>45816</v>
       </c>
@@ -102190,7 +102202,7 @@
         <v>16591</v>
       </c>
     </row>
-    <row r="91" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A91" s="31">
         <v>45816</v>
       </c>
@@ -102222,7 +102234,7 @@
         <v>16592</v>
       </c>
     </row>
-    <row r="92" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A92" s="31">
         <v>45816</v>
       </c>
@@ -102254,7 +102266,7 @@
         <v>16593</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A93" s="24">
         <v>45816</v>
       </c>
@@ -102283,7 +102295,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="94" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A94" s="31">
         <v>45816</v>
       </c>
@@ -102312,7 +102324,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="95" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A95" s="26">
         <v>45816</v>
       </c>
@@ -102341,7 +102353,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A96" s="24">
         <v>45816</v>
       </c>
@@ -102370,7 +102382,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A97" s="24">
         <v>45816</v>
       </c>
@@ -102402,7 +102414,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="98" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A98" s="31">
         <v>45816</v>
       </c>
@@ -102434,7 +102446,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="99" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A99" s="26">
         <v>45816</v>
       </c>
@@ -102466,7 +102478,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="100" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A100" s="29">
         <v>45817</v>
       </c>
@@ -102498,7 +102510,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="101" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A101" s="31">
         <v>45817</v>
       </c>
@@ -102530,7 +102542,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A102" s="24">
         <v>45817</v>
       </c>
@@ -102562,7 +102574,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="103" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A103" s="31">
         <v>45817</v>
       </c>
@@ -102594,7 +102606,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="104" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A104" s="31">
         <v>45817</v>
       </c>
@@ -102626,7 +102638,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="105" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A105" s="31">
         <v>45817</v>
       </c>
@@ -102658,7 +102670,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A106" s="24">
         <v>45817</v>
       </c>
@@ -102690,7 +102702,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="107" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A107" s="31">
         <v>45817</v>
       </c>
@@ -102722,7 +102734,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="108" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A108" s="29">
         <v>45817</v>
       </c>
@@ -102754,7 +102766,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A109" s="24">
         <v>45817</v>
       </c>
@@ -102786,7 +102798,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="110" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A110" s="31">
         <v>45817</v>
       </c>
@@ -102818,7 +102830,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A111" s="24">
         <v>45817</v>
       </c>
@@ -102847,7 +102859,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="112" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A112" s="31">
         <v>45817</v>
       </c>
@@ -102876,7 +102888,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="113" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A113" s="26">
         <v>45817</v>
       </c>
@@ -102905,7 +102917,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A114" s="24">
         <v>45817</v>
       </c>
@@ -102937,7 +102949,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="115" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A115" s="26">
         <v>45817</v>
       </c>
@@ -102969,7 +102981,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A116" s="24">
         <v>45817</v>
       </c>
@@ -103001,7 +103013,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A117" s="24">
         <v>45817</v>
       </c>
@@ -103033,7 +103045,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="118" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A118" s="28">
         <v>45817</v>
       </c>
@@ -103062,7 +103074,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="119" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A119" s="31">
         <v>45817</v>
       </c>
@@ -103094,7 +103106,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="120" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A120" s="31">
         <v>45817</v>
       </c>
@@ -103126,7 +103138,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="121" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A121" s="26">
         <v>45817</v>
       </c>
@@ -103158,7 +103170,7 @@
         <v>6031453.8099999996</v>
       </c>
     </row>
-    <row r="122" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A122" s="28">
         <v>45817</v>
       </c>
@@ -103187,7 +103199,7 @@
         <v>6031453.6699999999</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A123" s="24">
         <v>45817</v>
       </c>
@@ -103219,7 +103231,7 @@
         <v>6031453.6900000004</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A124" s="24">
         <v>45817</v>
       </c>
@@ -103251,7 +103263,7 @@
         <v>6031453.7000000002</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A125" s="24">
         <v>45817</v>
       </c>
@@ -103283,7 +103295,7 @@
         <v>6031453.75</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A126" s="24">
         <v>45817</v>
       </c>
@@ -103306,7 +103318,7 @@
         <v>4615003.93</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A127" s="24">
         <v>45817</v>
       </c>
@@ -103320,7 +103332,7 @@
         <v>16602</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A128" s="24">
         <v>45817</v>
       </c>
@@ -103352,7 +103364,7 @@
         <v>6031454.3700000001</v>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A129" s="24">
         <v>45817</v>
       </c>
@@ -103384,7 +103396,7 @@
         <v>6031454.7599999998</v>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A130" s="24">
         <v>45817</v>
       </c>
@@ -103416,7 +103428,7 @@
         <v>6031454.7599999998</v>
       </c>
     </row>
-    <row r="131" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A131" s="26">
         <v>45817</v>
       </c>
@@ -103448,7 +103460,7 @@
         <v>6031454.7599999998</v>
       </c>
     </row>
-    <row r="132" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A132" s="28">
         <v>45817</v>
       </c>
@@ -103477,7 +103489,7 @@
         <v>6031454.7699999996</v>
       </c>
     </row>
-    <row r="133" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A133" s="27">
         <v>45817</v>
       </c>
@@ -103509,7 +103521,7 @@
         <v>6031454.7800000003</v>
       </c>
     </row>
-    <row r="134" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A134" s="29">
         <v>45817</v>
       </c>
@@ -103541,7 +103553,7 @@
         <v>6031454.7699999996</v>
       </c>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A135" s="24">
         <v>45817</v>
       </c>
@@ -103573,7 +103585,7 @@
         <v>6031455.6100000003</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A136" s="24">
         <v>45817</v>
       </c>
@@ -103605,7 +103617,7 @@
         <v>6031455.6100000003</v>
       </c>
     </row>
-    <row r="137" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A137" s="26">
         <v>45817</v>
       </c>
@@ -103637,7 +103649,7 @@
         <v>6031455.5999999996</v>
       </c>
     </row>
-    <row r="138" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A138" s="31">
         <v>45817</v>
       </c>
@@ -103669,7 +103681,7 @@
         <v>6031455.6200000001</v>
       </c>
     </row>
-    <row r="139" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A139" s="26">
         <v>45817</v>
       </c>
@@ -103701,7 +103713,7 @@
         <v>6031456.7999999998</v>
       </c>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A140" s="24">
         <v>45817</v>
       </c>
@@ -103733,7 +103745,7 @@
         <v>6031456.8099999996</v>
       </c>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A141" s="24">
         <v>45817</v>
       </c>
@@ -103765,7 +103777,7 @@
         <v>6031456.8200000003</v>
       </c>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A142" s="24">
         <v>45817</v>
       </c>
@@ -103796,6 +103808,521 @@
       <c r="P142">
         <v>6031456.8300000001</v>
       </c>
+    </row>
+    <row r="143" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A143" s="42">
+        <v>45817</v>
+      </c>
+      <c r="B143" s="43">
+        <v>0.72431712962962957</v>
+      </c>
+      <c r="C143" s="44">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D143" s="44">
+        <v>-0.06</v>
+      </c>
+      <c r="E143" s="44" t="s">
+        <v>16642</v>
+      </c>
+      <c r="F143" s="44" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M143" s="44" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N143" s="44" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O143" s="44">
+        <v>325419.44</v>
+      </c>
+      <c r="P143" s="44">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
+    <row r="144" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A144" s="42">
+        <v>45817</v>
+      </c>
+      <c r="B144" s="43">
+        <v>0.72501157407407413</v>
+      </c>
+      <c r="C144" s="44">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D144" s="44">
+        <v>-0.06</v>
+      </c>
+      <c r="E144" s="44" t="s">
+        <v>16642</v>
+      </c>
+      <c r="F144" s="44" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M144" s="44" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N144" s="44" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O144" s="44">
+        <v>325419.44</v>
+      </c>
+      <c r="P144" s="44">
+        <v>6031442.8799999999</v>
+      </c>
+    </row>
+    <row r="145" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B145" s="2"/>
+    </row>
+    <row r="146" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B146" s="2"/>
+    </row>
+    <row r="147" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B147" s="2"/>
+    </row>
+    <row r="148" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B148" s="2"/>
+    </row>
+    <row r="149" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B149" s="2"/>
+    </row>
+    <row r="150" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B150" s="2"/>
+    </row>
+    <row r="151" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B151" s="2"/>
+    </row>
+    <row r="152" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B152" s="2"/>
+    </row>
+    <row r="153" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B153" s="2"/>
+    </row>
+    <row r="154" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B154" s="2"/>
+    </row>
+    <row r="155" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B155" s="2"/>
+    </row>
+    <row r="156" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B156" s="2"/>
+    </row>
+    <row r="157" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B157" s="2"/>
+    </row>
+    <row r="158" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B158" s="2"/>
+    </row>
+    <row r="159" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B159" s="2"/>
+    </row>
+    <row r="160" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B160" s="2"/>
+    </row>
+    <row r="161" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B161" s="2"/>
+    </row>
+    <row r="162" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B162" s="2"/>
+    </row>
+    <row r="163" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B163" s="2"/>
+    </row>
+    <row r="164" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B164" s="2"/>
+    </row>
+    <row r="165" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B165" s="2"/>
+    </row>
+    <row r="166" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B166" s="2"/>
+    </row>
+    <row r="167" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B167" s="2"/>
+    </row>
+    <row r="168" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B168" s="2"/>
+    </row>
+    <row r="169" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B169" s="2"/>
+    </row>
+    <row r="170" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B170" s="2"/>
+    </row>
+    <row r="171" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B171" s="2"/>
+    </row>
+    <row r="172" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B172" s="2"/>
+    </row>
+    <row r="173" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B173" s="2"/>
+    </row>
+    <row r="174" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B174" s="2"/>
+    </row>
+    <row r="175" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B175" s="2"/>
+    </row>
+    <row r="176" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B176" s="2"/>
+    </row>
+    <row r="177" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B177" s="2"/>
+    </row>
+    <row r="178" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B178" s="2"/>
+    </row>
+    <row r="179" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B179" s="2"/>
+    </row>
+    <row r="180" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B180" s="2"/>
+    </row>
+    <row r="181" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B181" s="2"/>
+    </row>
+    <row r="182" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B182" s="2"/>
+    </row>
+    <row r="183" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B183" s="2"/>
+    </row>
+    <row r="184" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B184" s="2"/>
+    </row>
+    <row r="185" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B185" s="2"/>
+    </row>
+    <row r="186" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B186" s="2"/>
+    </row>
+    <row r="187" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B187" s="2"/>
+    </row>
+    <row r="188" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B188" s="2"/>
+    </row>
+    <row r="189" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B189" s="2"/>
+    </row>
+    <row r="190" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B190" s="2"/>
+    </row>
+    <row r="191" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B191" s="2"/>
+    </row>
+    <row r="192" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B192" s="2"/>
+    </row>
+    <row r="193" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B193" s="2"/>
+    </row>
+    <row r="194" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B194" s="2"/>
+    </row>
+    <row r="195" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B195" s="2"/>
+    </row>
+    <row r="196" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B196" s="2"/>
+    </row>
+    <row r="197" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B197" s="2"/>
+    </row>
+    <row r="198" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B198" s="2"/>
+    </row>
+    <row r="199" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B199" s="2"/>
+    </row>
+    <row r="200" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B200" s="2"/>
+    </row>
+    <row r="201" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B201" s="2"/>
+    </row>
+    <row r="202" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B202" s="2"/>
+    </row>
+    <row r="203" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B203" s="2"/>
+    </row>
+    <row r="204" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B204" s="2"/>
+    </row>
+    <row r="205" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B205" s="2"/>
+    </row>
+    <row r="206" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B206" s="2"/>
+    </row>
+    <row r="207" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B207" s="2"/>
+    </row>
+    <row r="208" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B208" s="2"/>
+    </row>
+    <row r="209" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B209" s="2"/>
+    </row>
+    <row r="210" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B210" s="2"/>
+    </row>
+    <row r="211" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B211" s="2"/>
+    </row>
+    <row r="212" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B212" s="2"/>
+    </row>
+    <row r="213" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B213" s="2"/>
+    </row>
+    <row r="214" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B214" s="2"/>
+    </row>
+    <row r="215" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B215" s="2"/>
+    </row>
+    <row r="216" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B216" s="2"/>
+    </row>
+    <row r="217" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B217" s="2"/>
+    </row>
+    <row r="218" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B218" s="2"/>
+    </row>
+    <row r="219" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B219" s="2"/>
+    </row>
+    <row r="220" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B220" s="2"/>
+    </row>
+    <row r="221" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B221" s="2"/>
+    </row>
+    <row r="222" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B222" s="2"/>
+    </row>
+    <row r="223" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B223" s="2"/>
+    </row>
+    <row r="224" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B224" s="2"/>
+    </row>
+    <row r="225" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B225" s="2"/>
+    </row>
+    <row r="226" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B226" s="2"/>
+    </row>
+    <row r="227" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B227" s="2"/>
+    </row>
+    <row r="228" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B228" s="2"/>
+    </row>
+    <row r="229" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B229" s="2"/>
+    </row>
+    <row r="230" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B230" s="2"/>
+    </row>
+    <row r="231" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B231" s="2"/>
+    </row>
+    <row r="232" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B232" s="2"/>
+    </row>
+    <row r="233" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B233" s="2"/>
+    </row>
+    <row r="234" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B234" s="2"/>
+    </row>
+    <row r="235" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B235" s="2"/>
+    </row>
+    <row r="236" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B236" s="2"/>
+    </row>
+    <row r="237" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B237" s="2"/>
+    </row>
+    <row r="238" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B238" s="2"/>
+    </row>
+    <row r="239" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B239" s="2"/>
+    </row>
+    <row r="240" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B240" s="2"/>
+    </row>
+    <row r="241" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B241" s="2"/>
+    </row>
+    <row r="242" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B242" s="2"/>
+    </row>
+    <row r="243" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B243" s="2"/>
+    </row>
+    <row r="244" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B244" s="2"/>
+    </row>
+    <row r="245" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B245" s="2"/>
+    </row>
+    <row r="246" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B246" s="2"/>
+    </row>
+    <row r="247" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B247" s="2"/>
+    </row>
+    <row r="248" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B248" s="2"/>
+    </row>
+    <row r="249" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B249" s="2"/>
+    </row>
+    <row r="250" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B250" s="2"/>
+    </row>
+    <row r="251" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B251" s="2"/>
+    </row>
+    <row r="252" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B252" s="2"/>
+    </row>
+    <row r="253" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B253" s="2"/>
+    </row>
+    <row r="254" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B254" s="2"/>
+    </row>
+    <row r="255" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B255" s="2"/>
+    </row>
+    <row r="256" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B256" s="2"/>
+    </row>
+    <row r="257" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B257" s="2"/>
+    </row>
+    <row r="258" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B258" s="2"/>
+    </row>
+    <row r="259" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B259" s="2"/>
+    </row>
+    <row r="260" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B260" s="2"/>
+    </row>
+    <row r="261" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B261" s="2"/>
+    </row>
+    <row r="262" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B262" s="2"/>
+    </row>
+    <row r="263" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B263" s="2"/>
+    </row>
+    <row r="264" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B264" s="2"/>
+    </row>
+    <row r="265" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B265" s="2"/>
+    </row>
+    <row r="266" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B266" s="2"/>
+    </row>
+    <row r="267" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B267" s="2"/>
+    </row>
+    <row r="268" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B268" s="2"/>
+    </row>
+    <row r="269" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B269" s="2"/>
+    </row>
+    <row r="270" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B270" s="2"/>
+    </row>
+    <row r="271" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B271" s="2"/>
+    </row>
+    <row r="272" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B272" s="2"/>
+    </row>
+    <row r="273" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B273" s="2"/>
+    </row>
+    <row r="274" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B274" s="2"/>
+    </row>
+    <row r="275" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B275" s="2"/>
+    </row>
+    <row r="276" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B276" s="2"/>
+    </row>
+    <row r="277" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B277" s="2"/>
+    </row>
+    <row r="278" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B278" s="2"/>
+    </row>
+    <row r="279" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B279" s="2"/>
+    </row>
+    <row r="280" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B280" s="2"/>
+    </row>
+    <row r="281" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B281" s="2"/>
+    </row>
+    <row r="282" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B282" s="2"/>
+    </row>
+    <row r="283" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B283" s="2"/>
+    </row>
+    <row r="284" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B284" s="2"/>
+    </row>
+    <row r="285" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B285" s="2"/>
+    </row>
+    <row r="286" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B286" s="2"/>
+    </row>
+    <row r="287" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B287" s="2"/>
+    </row>
+    <row r="288" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B288" s="2"/>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B289" s="2"/>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B290" s="2"/>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B291" s="2"/>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B292" s="2"/>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B293" s="2"/>
+    </row>
+    <row r="294" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A294" s="42"/>
+      <c r="B294" s="43"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
KP functionality added: now it is comparing the current KP with the last KP written in the log excel to substract the progress.
</commit_message>
<xml_diff>
--- a/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
+++ b/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\PYTHON\Vicente\Online-Log-Development\Excel TEmplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6FAD60-529C-4391-A7FF-87ACB125A19C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CE7858-E5B2-4309-A7AF-371EC304CD21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="42870" yWindow="6670" windowWidth="32140" windowHeight="16720" xr2:uid="{1722F03E-A338-4BDB-920F-BA87EA8992B5}"/>
+    <workbookView xWindow="1260" yWindow="1780" windowWidth="32140" windowHeight="16720" xr2:uid="{1722F03E-A338-4BDB-920F-BA87EA8992B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17026" uniqueCount="16645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17082" uniqueCount="16648">
   <si>
     <t>Date</t>
   </si>
@@ -49971,6 +49971,15 @@
   </si>
   <si>
     <t>ROV Off Deck</t>
+  </si>
+  <si>
+    <t>Current KP: 0.006 | First hourly log</t>
+  </si>
+  <si>
+    <t>cdfffsdf</t>
+  </si>
+  <si>
+    <t>Current KP: 0.006 | Progress last hour: +0.000 km</t>
   </si>
 </sst>
 </file>
@@ -50473,11 +50482,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E3A69F-5804-46B3-8092-81B33E8A06FF}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:XFD294"/>
+  <dimension ref="A1:XFD287"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E146" sqref="E146"/>
+      <selection pane="bottomLeft" activeCell="D157" sqref="D157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -104051,85 +104060,491 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B150" s="2"/>
+    <row r="150" spans="1:17" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A150" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B150" s="46">
+        <v>0.85487268518518522</v>
+      </c>
+      <c r="C150" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D150" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E150" s="47" t="s">
+        <v>16645</v>
+      </c>
+      <c r="F150" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M150" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N150" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O150" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P150" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B151" s="2"/>
+      <c r="A151" s="24">
+        <v>45817</v>
+      </c>
+      <c r="B151" s="2">
+        <v>0.85487268518518522</v>
+      </c>
+      <c r="C151">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D151">
+        <v>-0.06</v>
+      </c>
+      <c r="E151" t="s">
+        <v>16646</v>
+      </c>
+      <c r="F151" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M151" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N151" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O151">
+        <v>325419.44</v>
+      </c>
+      <c r="P151">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
     <row r="152" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B152" s="2"/>
+      <c r="A152" s="24">
+        <v>45817</v>
+      </c>
+      <c r="B152" s="2">
+        <v>0.85502314814814817</v>
+      </c>
+      <c r="C152">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D152">
+        <v>-0.06</v>
+      </c>
+      <c r="E152" t="s">
+        <v>16644</v>
+      </c>
+      <c r="F152" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M152" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N152" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O152">
+        <v>325419.44</v>
+      </c>
+      <c r="P152">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B153" s="2"/>
+      <c r="A153" s="24">
+        <v>45817</v>
+      </c>
+      <c r="B153" s="2">
+        <v>0.85516203703703708</v>
+      </c>
+      <c r="C153">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D153">
+        <v>-0.06</v>
+      </c>
+      <c r="E153" t="s">
+        <v>16644</v>
+      </c>
+      <c r="F153" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M153" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N153" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O153">
+        <v>325419.44</v>
+      </c>
+      <c r="P153">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B154" s="2"/>
+    <row r="154" spans="1:17" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A154" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B154" s="46">
+        <v>0.85556712962962966</v>
+      </c>
+      <c r="C154" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D154" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E154" s="47" t="s">
+        <v>16645</v>
+      </c>
+      <c r="F154" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M154" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N154" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O154" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P154" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
     <row r="155" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B155" s="2"/>
+      <c r="A155" s="24">
+        <v>45817</v>
+      </c>
+      <c r="B155" s="2">
+        <v>0.86984953703703705</v>
+      </c>
+      <c r="C155">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D155">
+        <v>-0.06</v>
+      </c>
+      <c r="E155" t="s">
+        <v>16644</v>
+      </c>
+      <c r="F155" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M155" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N155" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O155">
+        <v>325419.44</v>
+      </c>
+      <c r="P155">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B156" s="2"/>
+    <row r="156" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A156" s="26">
+        <v>45817</v>
+      </c>
+      <c r="B156" s="5">
+        <v>0.86987268518518523</v>
+      </c>
+      <c r="C156" s="6">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D156" s="6">
+        <v>-0.06</v>
+      </c>
+      <c r="E156" s="6" t="s">
+        <v>16383</v>
+      </c>
+      <c r="F156" s="6" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M156" s="6" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N156" s="6" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O156" s="6">
+        <v>325419.44</v>
+      </c>
+      <c r="P156" s="6">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B157" s="2"/>
+    <row r="157" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A157" s="27">
+        <v>45817</v>
+      </c>
+      <c r="B157" s="7">
+        <v>0.86988425925925927</v>
+      </c>
+      <c r="C157" s="8">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D157" s="8">
+        <v>-0.06</v>
+      </c>
+      <c r="E157" s="8" t="s">
+        <v>16384</v>
+      </c>
+      <c r="F157" s="8" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M157" s="8" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N157" s="8" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O157" s="8">
+        <v>325419.44</v>
+      </c>
+      <c r="P157" s="8">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B158" s="2"/>
+    <row r="158" spans="1:17" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A158" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B158" s="46">
+        <v>0.87015046296296295</v>
+      </c>
+      <c r="C158" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D158" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E158" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F158" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M158" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N158" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O158" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P158" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B159" s="2"/>
+    <row r="159" spans="1:17" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A159" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B159" s="46">
+        <v>0.87084490740740739</v>
+      </c>
+      <c r="C159" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D159" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E159" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F159" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M159" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N159" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O159" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P159" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B160" s="2"/>
+    <row r="160" spans="1:17" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A160" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B160" s="46">
+        <v>0.87153935185185183</v>
+      </c>
+      <c r="C160" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D160" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E160" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F160" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M160" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N160" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O160" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P160" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B161" s="2"/>
+    <row r="161" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A161" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B161" s="46">
+        <v>0.87223379629629627</v>
+      </c>
+      <c r="C161" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D161" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E161" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F161" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M161" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N161" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O161" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P161" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B162" s="2"/>
+    <row r="162" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A162" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B162" s="46">
+        <v>0.87292824074074071</v>
+      </c>
+      <c r="C162" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D162" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E162" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F162" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M162" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N162" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O162" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P162" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B163" s="2"/>
+    <row r="163" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A163" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B163" s="46">
+        <v>0.87362268518518515</v>
+      </c>
+      <c r="C163" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D163" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E163" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F163" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M163" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N163" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O163" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P163" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B164" s="2"/>
     </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B165" s="2"/>
     </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B166" s="2"/>
     </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B167" s="2"/>
     </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B168" s="2"/>
     </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B169" s="2"/>
     </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B170" s="2"/>
     </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B171" s="2"/>
     </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B172" s="2"/>
     </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B173" s="2"/>
     </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B174" s="2"/>
     </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B175" s="2"/>
     </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B176" s="2"/>
     </row>
     <row r="177" spans="2:2" x14ac:dyDescent="0.35">
@@ -104420,72 +104835,51 @@
     <row r="272" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B272" s="2"/>
     </row>
-    <row r="273" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B273" s="2"/>
     </row>
-    <row r="274" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B274" s="2"/>
     </row>
-    <row r="275" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B275" s="2"/>
     </row>
-    <row r="276" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B276" s="2"/>
     </row>
-    <row r="277" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B277" s="2"/>
     </row>
-    <row r="278" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B278" s="2"/>
     </row>
-    <row r="279" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B279" s="2"/>
     </row>
-    <row r="280" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B280" s="2"/>
     </row>
-    <row r="281" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B281" s="2"/>
     </row>
-    <row r="282" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B282" s="2"/>
     </row>
-    <row r="283" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B283" s="2"/>
     </row>
-    <row r="284" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B284" s="2"/>
     </row>
-    <row r="285" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B285" s="2"/>
     </row>
-    <row r="286" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B286" s="2"/>
     </row>
-    <row r="287" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B287" s="2"/>
-    </row>
-    <row r="288" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B288" s="2"/>
-    </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B289" s="2"/>
-    </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B290" s="2"/>
-    </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B291" s="2"/>
-    </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B292" s="2"/>
-    </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B293" s="2"/>
-    </row>
-    <row r="294" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A294" s="42"/>
-      <c r="B294" s="43"/>
+    <row r="287" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A287" s="42"/>
+      <c r="B287" s="43"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Buttons have background color now. Tkinter them was changed from 'vista' to 'clam'
Some bugs were fixed to make it work
</commit_message>
<xml_diff>
--- a/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
+++ b/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\PYTHON\Vicente\Online-Log-Development\Excel TEmplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CE7858-E5B2-4309-A7AF-371EC304CD21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CC5259-E92F-42E2-86AA-9C28D9ABF037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1260" yWindow="1780" windowWidth="32140" windowHeight="16720" xr2:uid="{1722F03E-A338-4BDB-920F-BA87EA8992B5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17082" uniqueCount="16648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17154" uniqueCount="16648">
   <si>
     <t>Date</t>
   </si>
@@ -104508,91 +104508,613 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="164" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B164" s="2"/>
+    <row r="164" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A164" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B164" s="46">
+        <v>0.8743171296296296</v>
+      </c>
+      <c r="C164" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D164" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E164" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F164" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M164" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N164" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O164" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P164" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="165" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B165" s="2"/>
+    <row r="165" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A165" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B165" s="46">
+        <v>0.87570601851851848</v>
+      </c>
+      <c r="C165" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D165" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E165" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F165" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M165" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N165" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O165" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P165" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="166" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B166" s="2"/>
+    <row r="166" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A166" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B166" s="46">
+        <v>0.87640046296296292</v>
+      </c>
+      <c r="C166" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D166" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E166" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F166" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M166" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N166" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O166" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P166" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="167" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B167" s="2"/>
+    <row r="167" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A167" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B167" s="46">
+        <v>0.87709490740740736</v>
+      </c>
+      <c r="C167" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D167" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E167" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F167" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M167" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N167" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O167" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P167" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="168" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B168" s="2"/>
+    <row r="168" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A168" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B168" s="46">
+        <v>0.87778935185185181</v>
+      </c>
+      <c r="C168" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D168" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E168" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F168" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M168" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N168" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O168" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P168" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="169" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B169" s="2"/>
+    <row r="169" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A169" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B169" s="46">
+        <v>0.87848379629629625</v>
+      </c>
+      <c r="C169" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D169" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E169" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F169" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M169" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N169" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O169" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P169" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="170" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B170" s="2"/>
+    <row r="170" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A170" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B170" s="46">
+        <v>0.87987268518518513</v>
+      </c>
+      <c r="C170" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D170" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E170" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F170" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M170" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N170" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O170" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P170" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="171" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B171" s="2"/>
+    <row r="171" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A171" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B171" s="46">
+        <v>0.88265046296296301</v>
+      </c>
+      <c r="C171" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D171" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E171" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F171" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M171" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N171" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O171" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P171" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="172" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B172" s="2"/>
+    <row r="172" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A172" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B172" s="46">
+        <v>0.88334490740740745</v>
+      </c>
+      <c r="C172" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D172" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E172" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F172" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M172" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N172" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O172" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P172" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="173" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B173" s="2"/>
+    <row r="173" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A173" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B173" s="46">
+        <v>0.8840393518518519</v>
+      </c>
+      <c r="C173" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D173" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E173" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F173" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M173" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N173" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O173" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P173" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="174" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B174" s="2"/>
+    <row r="174" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A174" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B174" s="46">
+        <v>0.88473379629629634</v>
+      </c>
+      <c r="C174" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D174" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E174" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F174" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M174" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N174" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O174" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P174" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="175" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B175" s="2"/>
+    <row r="175" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A175" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B175" s="46">
+        <v>0.88542824074074078</v>
+      </c>
+      <c r="C175" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D175" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E175" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F175" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M175" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N175" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O175" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P175" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="176" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B176" s="2"/>
+    <row r="176" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A176" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B176" s="46">
+        <v>0.88612268518518522</v>
+      </c>
+      <c r="C176" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D176" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E176" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F176" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M176" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N176" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O176" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P176" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B177" s="2"/>
+    <row r="177" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A177" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B177" s="46">
+        <v>0.88820601851851855</v>
+      </c>
+      <c r="C177" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D177" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E177" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F177" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M177" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N177" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O177" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P177" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B178" s="2"/>
+    <row r="178" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A178" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B178" s="46">
+        <v>0.89098379629629632</v>
+      </c>
+      <c r="C178" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D178" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E178" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F178" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M178" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N178" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O178" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P178" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B179" s="2"/>
+    <row r="179" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A179" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B179" s="46">
+        <v>0.89445601851851853</v>
+      </c>
+      <c r="C179" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D179" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E179" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F179" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M179" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N179" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O179" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P179" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B180" s="2"/>
+    <row r="180" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A180" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B180" s="46">
+        <v>0.89515046296296297</v>
+      </c>
+      <c r="C180" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D180" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E180" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F180" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M180" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N180" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O180" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P180" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B181" s="2"/>
+    <row r="181" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A181" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B181" s="46">
+        <v>0.89723379629629629</v>
+      </c>
+      <c r="C181" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D181" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E181" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F181" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M181" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N181" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O181" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P181" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B182" s="2"/>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B183" s="2"/>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B184" s="2"/>
     </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B185" s="2"/>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B186" s="2"/>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B187" s="2"/>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B188" s="2"/>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B189" s="2"/>
     </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B190" s="2"/>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B191" s="2"/>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B192" s="2"/>
     </row>
     <row r="193" spans="2:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Bug fixed: the custom colors defined by user were overwritten y the settings menu when Save and Close was pressed.
</commit_message>
<xml_diff>
--- a/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
+++ b/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\PYTHON\Vicente\Online-Log-Development\Excel TEmplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CC5259-E92F-42E2-86AA-9C28D9ABF037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A49DCB8-D4CF-4110-BE4F-49C52EB16902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="1780" windowWidth="32140" windowHeight="16720" xr2:uid="{1722F03E-A338-4BDB-920F-BA87EA8992B5}"/>
+    <workbookView minimized="1" xWindow="1260" yWindow="1780" windowWidth="32140" windowHeight="16720" xr2:uid="{1722F03E-A338-4BDB-920F-BA87EA8992B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17154" uniqueCount="16648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17278" uniqueCount="16648">
   <si>
     <t>Date</t>
   </si>
@@ -50485,7 +50485,7 @@
   <dimension ref="A1:XFD287"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D157" sqref="D157"/>
     </sheetView>
   </sheetViews>
@@ -105084,133 +105084,1032 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="182" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B182" s="2"/>
+    <row r="182" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A182" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B182" s="46">
+        <v>0.89792824074074074</v>
+      </c>
+      <c r="C182" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D182" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E182" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F182" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M182" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N182" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O182" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P182" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="183" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B183" s="2"/>
+    <row r="183" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A183" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B183" s="46">
+        <v>0.89862268518518518</v>
+      </c>
+      <c r="C183" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D183" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E183" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F183" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M183" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N183" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O183" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P183" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="184" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B184" s="2"/>
+    <row r="184" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A184" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B184" s="46">
+        <v>0.90417824074074071</v>
+      </c>
+      <c r="C184" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D184" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E184" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F184" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M184" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N184" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O184" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P184" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="185" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B185" s="2"/>
+    <row r="185" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A185" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B185" s="46">
+        <v>0.90487268518518515</v>
+      </c>
+      <c r="C185" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D185" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E185" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F185" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M185" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N185" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O185" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P185" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="186" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B186" s="2"/>
+    <row r="186" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A186" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B186" s="46">
+        <v>0.91876157407407411</v>
+      </c>
+      <c r="C186" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D186" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E186" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F186" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M186" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N186" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O186" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P186" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="187" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B187" s="2"/>
+    <row r="187" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A187" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B187" s="46">
+        <v>0.91945601851851855</v>
+      </c>
+      <c r="C187" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D187" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E187" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F187" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M187" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N187" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O187" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P187" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="188" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B188" s="2"/>
+    <row r="188" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A188" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B188" s="46">
+        <v>0.92015046296296299</v>
+      </c>
+      <c r="C188" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D188" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E188" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F188" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M188" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N188" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O188" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P188" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="189" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B189" s="2"/>
+    <row r="189" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A189" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B189" s="46">
+        <v>0.92084490740740743</v>
+      </c>
+      <c r="C189" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D189" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E189" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F189" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M189" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N189" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O189" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P189" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="190" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B190" s="2"/>
+    <row r="190" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A190" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B190" s="46">
+        <v>0.92153935185185187</v>
+      </c>
+      <c r="C190" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D190" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E190" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F190" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M190" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N190" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O190" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P190" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="191" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B191" s="2"/>
+    <row r="191" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A191" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B191" s="46">
+        <v>0.92223379629629632</v>
+      </c>
+      <c r="C191" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D191" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E191" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F191" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M191" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N191" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O191" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P191" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="192" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B192" s="2"/>
+    <row r="192" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A192" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B192" s="46">
+        <v>0.92292824074074076</v>
+      </c>
+      <c r="C192" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D192" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E192" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F192" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M192" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N192" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O192" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P192" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B193" s="2"/>
+    <row r="193" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A193" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B193" s="46">
+        <v>0.9236226851851852</v>
+      </c>
+      <c r="C193" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D193" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E193" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F193" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M193" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N193" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O193" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P193" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B194" s="2"/>
+    <row r="194" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A194" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B194" s="46">
+        <v>0.92431712962962964</v>
+      </c>
+      <c r="C194" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D194" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E194" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F194" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M194" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N194" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O194" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P194" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B195" s="2"/>
+    <row r="195" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A195" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B195" s="46">
+        <v>0.92501157407407408</v>
+      </c>
+      <c r="C195" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D195" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E195" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F195" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M195" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N195" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O195" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P195" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B196" s="2"/>
+    <row r="196" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A196" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B196" s="46">
+        <v>0.92570601851851853</v>
+      </c>
+      <c r="C196" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D196" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E196" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F196" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M196" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N196" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O196" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P196" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B197" s="2"/>
+    <row r="197" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A197" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B197" s="46">
+        <v>0.92640046296296297</v>
+      </c>
+      <c r="C197" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D197" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E197" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F197" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M197" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N197" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O197" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P197" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B198" s="2"/>
+    <row r="198" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A198" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B198" s="46">
+        <v>0.92709490740740741</v>
+      </c>
+      <c r="C198" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D198" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E198" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F198" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M198" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N198" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O198" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P198" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B199" s="2"/>
+    <row r="199" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A199" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B199" s="46">
+        <v>0.92778935185185185</v>
+      </c>
+      <c r="C199" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D199" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E199" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F199" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M199" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N199" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O199" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P199" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B200" s="2"/>
+    <row r="200" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A200" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B200" s="46">
+        <v>0.92848379629629629</v>
+      </c>
+      <c r="C200" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D200" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E200" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F200" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M200" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N200" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O200" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P200" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="201" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B201" s="2"/>
+    <row r="201" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A201" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B201" s="46">
+        <v>0.92917824074074074</v>
+      </c>
+      <c r="C201" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D201" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E201" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F201" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M201" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N201" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O201" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P201" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B202" s="2"/>
+    <row r="202" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A202" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B202" s="46">
+        <v>0.92987268518518518</v>
+      </c>
+      <c r="C202" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D202" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E202" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F202" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M202" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N202" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O202" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P202" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B203" s="2"/>
+    <row r="203" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A203" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B203" s="46">
+        <v>0.93056712962962962</v>
+      </c>
+      <c r="C203" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D203" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E203" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F203" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M203" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N203" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O203" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P203" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="204" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B204" s="2"/>
+    <row r="204" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A204" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B204" s="46">
+        <v>0.93126157407407406</v>
+      </c>
+      <c r="C204" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D204" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E204" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F204" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M204" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N204" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O204" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P204" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="205" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B205" s="2"/>
+    <row r="205" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A205" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B205" s="46">
+        <v>0.9319560185185185</v>
+      </c>
+      <c r="C205" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D205" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E205" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F205" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M205" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N205" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O205" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P205" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="206" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B206" s="2"/>
+    <row r="206" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A206" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B206" s="46">
+        <v>0.93265046296296295</v>
+      </c>
+      <c r="C206" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D206" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E206" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F206" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M206" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N206" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O206" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P206" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="207" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B207" s="2"/>
+    <row r="207" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A207" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B207" s="46">
+        <v>0.94167824074074069</v>
+      </c>
+      <c r="C207" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D207" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E207" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F207" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M207" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N207" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O207" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P207" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="208" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B208" s="2"/>
+    <row r="208" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A208" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B208" s="46">
+        <v>0.94237268518518513</v>
+      </c>
+      <c r="C208" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D208" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E208" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F208" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M208" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N208" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O208" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P208" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B209" s="2"/>
+    <row r="209" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A209" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B209" s="46">
+        <v>0.94306712962962957</v>
+      </c>
+      <c r="C209" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D209" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E209" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F209" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M209" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N209" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O209" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P209" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B210" s="2"/>
+    <row r="210" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A210" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B210" s="46">
+        <v>0.94376157407407413</v>
+      </c>
+      <c r="C210" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D210" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E210" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F210" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M210" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N210" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O210" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P210" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B211" s="2"/>
+    <row r="211" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A211" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B211" s="46">
+        <v>0.94445601851851857</v>
+      </c>
+      <c r="C211" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D211" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E211" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F211" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M211" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N211" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O211" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P211" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="212" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B212" s="2"/>
+    <row r="212" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A212" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B212" s="46">
+        <v>0.94515046296296301</v>
+      </c>
+      <c r="C212" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D212" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E212" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F212" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M212" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N212" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O212" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P212" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="213" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B213" s="2"/>
     </row>
-    <row r="214" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B214" s="2"/>
     </row>
-    <row r="215" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B215" s="2"/>
     </row>
-    <row r="216" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B216" s="2"/>
     </row>
-    <row r="217" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B217" s="2"/>
     </row>
-    <row r="218" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B218" s="2"/>
     </row>
-    <row r="219" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B219" s="2"/>
     </row>
-    <row r="220" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B220" s="2"/>
     </row>
-    <row r="221" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B221" s="2"/>
     </row>
-    <row r="222" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B222" s="2"/>
     </row>
-    <row r="223" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B223" s="2"/>
     </row>
-    <row r="224" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B224" s="2"/>
     </row>
     <row r="225" spans="2:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Custom color tab removed from settings menu
</commit_message>
<xml_diff>
--- a/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
+++ b/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\PYTHON\Vicente\Online-Log-Development\Excel TEmplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A49DCB8-D4CF-4110-BE4F-49C52EB16902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63384DD-778A-42C5-AB95-E23A7D09BCCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView minimized="1" xWindow="1260" yWindow="1780" windowWidth="32140" windowHeight="16720" xr2:uid="{1722F03E-A338-4BDB-920F-BA87EA8992B5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17278" uniqueCount="16648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17294" uniqueCount="16648">
   <si>
     <t>Date</t>
   </si>
@@ -50485,7 +50485,7 @@
   <dimension ref="A1:XFD287"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D157" sqref="D157"/>
     </sheetView>
   </sheetViews>
@@ -106076,17 +106076,133 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="213" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B213" s="2"/>
+    <row r="213" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A213" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B213" s="46">
+        <v>0.94584490740740745</v>
+      </c>
+      <c r="C213" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D213" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E213" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F213" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M213" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N213" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O213" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P213" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="214" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B214" s="2"/>
+    <row r="214" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A214" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B214" s="46">
+        <v>0.9465393518518519</v>
+      </c>
+      <c r="C214" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D214" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E214" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F214" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M214" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N214" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O214" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P214" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="215" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B215" s="2"/>
+    <row r="215" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A215" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B215" s="46">
+        <v>0.94723379629629634</v>
+      </c>
+      <c r="C215" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D215" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E215" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F215" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M215" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N215" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O215" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P215" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
-    <row r="216" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B216" s="2"/>
+    <row r="216" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A216" s="45">
+        <v>45817</v>
+      </c>
+      <c r="B216" s="46">
+        <v>0.94792824074074078</v>
+      </c>
+      <c r="C216" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D216" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E216" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F216" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M216" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N216" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O216" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P216" s="47">
+        <v>6031442.8799999999</v>
+      </c>
     </row>
     <row r="217" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B217" s="2"/>

</xml_diff>

<commit_message>
save_excel() function updated to fill in 600053_Daily_Log-Week24.xlsb according to standar template: - The Excel Log search is based finding this strings in the header (it ignores capital letters): {'runline', 'kp', 'kp ref.', 'event', 'guid'} - GUID replaced RecordID - Browser dialog modified to show .xlsb files as well
</commit_message>
<xml_diff>
--- a/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
+++ b/Excel TEmplate/Rheinemtall_SampleTestLog_v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\PYTHON\Vicente\Online-Log-Development\Excel TEmplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\PYTHON\Vicente\Online-Log-Development\Excel Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7817A5-2E94-4FFB-956E-3A824B892FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EFC335-ED2F-405A-B2BF-FFBA3684E003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{1722F03E-A338-4BDB-920F-BA87EA8992B5}"/>
+    <workbookView xWindow="3800" yWindow="3800" windowWidth="32140" windowHeight="16720" xr2:uid="{1722F03E-A338-4BDB-920F-BA87EA8992B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17382" uniqueCount="16648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17392" uniqueCount="16650">
   <si>
     <t>Date</t>
   </si>
@@ -49980,6 +49980,12 @@
   </si>
   <si>
     <t>Current KP: 0.006 | Progress last hour: +0.000 km</t>
+  </si>
+  <si>
+    <t>8af75ff5-6dde-4b78-9c9b-9617cd65db38</t>
+  </si>
+  <si>
+    <t>ee75e21b-be40-46c8-b985-243ccc8fae28</t>
   </si>
 </sst>
 </file>
@@ -50098,7 +50104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -50147,6 +50153,7 @@
     <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="21" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -50484,8 +50491,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:XFD287"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A184" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D157" sqref="D157"/>
     </sheetView>
   </sheetViews>
@@ -106460,7 +106467,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="225" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:17" s="47" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A225" s="45">
         <v>45817</v>
       </c>
@@ -106492,7 +106499,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="226" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:17" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A226" s="42">
         <v>45818</v>
       </c>
@@ -106524,7 +106531,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="227" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:17" s="47" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A227" s="45">
         <v>45818</v>
       </c>
@@ -106556,7 +106563,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="228" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:17" s="47" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A228" s="45">
         <v>45818</v>
       </c>
@@ -106588,7 +106595,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="229" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:17" s="47" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A229" s="45">
         <v>45818</v>
       </c>
@@ -106620,7 +106627,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="230" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:17" s="47" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A230" s="45">
         <v>45818</v>
       </c>
@@ -106652,7 +106659,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="231" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:17" s="47" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A231" s="45">
         <v>45818</v>
       </c>
@@ -106684,7 +106691,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="232" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:17" s="47" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A232" s="45">
         <v>45818</v>
       </c>
@@ -106716,7 +106723,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="233" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:17" s="47" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A233" s="45">
         <v>45818</v>
       </c>
@@ -106748,7 +106755,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="234" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:17" s="47" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A234" s="45">
         <v>45818</v>
       </c>
@@ -106780,7 +106787,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="235" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:17" s="47" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A235" s="45">
         <v>45818</v>
       </c>
@@ -106812,7 +106819,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="236" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:17" s="47" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A236" s="45">
         <v>45818</v>
       </c>
@@ -106844,7 +106851,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="237" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:17" s="47" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A237" s="45">
         <v>45818</v>
       </c>
@@ -106876,7 +106883,7 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="238" spans="1:16" s="47" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:17" s="47" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A238" s="45">
         <v>45818</v>
       </c>
@@ -106908,11 +106915,75 @@
         <v>6031442.8799999999</v>
       </c>
     </row>
-    <row r="239" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B239" s="2"/>
+    <row r="239" spans="1:17" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A239" s="45">
+        <v>45818</v>
+      </c>
+      <c r="B239" s="46">
+        <v>0.62501157407407404</v>
+      </c>
+      <c r="C239" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D239" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E239" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F239" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M239" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N239" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O239" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P239" s="47">
+        <v>6031442.8799999999</v>
+      </c>
+      <c r="Q239" s="48" t="s">
+        <v>16648</v>
+      </c>
     </row>
-    <row r="240" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B240" s="2"/>
+    <row r="240" spans="1:17" s="47" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A240" s="45">
+        <v>45818</v>
+      </c>
+      <c r="B240" s="46">
+        <v>0.66667824074074078</v>
+      </c>
+      <c r="C240" s="47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D240" s="47">
+        <v>-0.06</v>
+      </c>
+      <c r="E240" s="47" t="s">
+        <v>16647</v>
+      </c>
+      <c r="F240" s="47" t="s">
+        <v>16581</v>
+      </c>
+      <c r="M240" s="47" t="s">
+        <v>16582</v>
+      </c>
+      <c r="N240" s="47" t="s">
+        <v>16583</v>
+      </c>
+      <c r="O240" s="47">
+        <v>325419.44</v>
+      </c>
+      <c r="P240" s="47">
+        <v>6031442.8799999999</v>
+      </c>
+      <c r="Q240" s="48" t="s">
+        <v>16649</v>
+      </c>
     </row>
     <row r="241" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B241" s="2"/>

</xml_diff>